<commit_message>
ajout flag break for avoid duplicating
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t xml:space="preserve">LIGNE </t>
   </si>
@@ -119,14 +119,21 @@
   </si>
   <si>
     <t>VOIR README</t>
+  </si>
+  <si>
+    <t>MRTRAM</t>
+  </si>
+  <si>
+    <t>SEMALY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh:\ mm:\ ss"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -248,7 +255,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -273,6 +280,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
@@ -580,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,10 +693,6 @@
         <f>D4/F4</f>
         <v>0.95217306567920479</v>
       </c>
-      <c r="I4" s="7">
-        <f>H4/86400</f>
-        <v>0</v>
-      </c>
       <c r="L4">
         <f t="shared" ref="L4:L14" si="2">J4+K4</f>
         <v>0</v>
@@ -723,7 +727,7 @@
         <v>13000</v>
       </c>
       <c r="I5" s="7">
-        <f t="shared" ref="I5:I29" si="4">H5/86400</f>
+        <f t="shared" ref="I5:I30" si="4">H5/86400</f>
         <v>0.15046296296296297</v>
       </c>
       <c r="J5">
@@ -811,10 +815,6 @@
         <f t="shared" si="3"/>
         <v>0.92751631741669527</v>
       </c>
-      <c r="I7" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L7">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -845,10 +845,6 @@
         <f>D8/F8</f>
         <v>0.4597927658762952</v>
       </c>
-      <c r="I8" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -879,10 +875,6 @@
         <f>D9/F9</f>
         <v>0.9005573481959519</v>
       </c>
-      <c r="I9" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L9">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -913,10 +905,6 @@
         <f t="shared" si="3"/>
         <v>0.9863494539781591</v>
       </c>
-      <c r="I10" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L10">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -947,10 +935,6 @@
         <f t="shared" si="3"/>
         <v>0.88636363636363635</v>
       </c>
-      <c r="I11" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -981,10 +965,6 @@
         <f t="shared" si="3"/>
         <v>0.93073329270769856</v>
       </c>
-      <c r="I12" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L12">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1015,10 +995,6 @@
         <f t="shared" si="3"/>
         <v>0.9699453551912568</v>
       </c>
-      <c r="I13" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L13">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1049,10 +1025,6 @@
         <f t="shared" si="3"/>
         <v>0.93324287652645865</v>
       </c>
-      <c r="I14" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L14">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1177,10 +1149,6 @@
         <f t="shared" si="3"/>
         <v>0.98027937551355793</v>
       </c>
-      <c r="I17" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L17">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -1211,10 +1179,6 @@
         <f t="shared" si="3"/>
         <v>0.76106018333997605</v>
       </c>
-      <c r="I18" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L18">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -1245,10 +1209,6 @@
         <f t="shared" si="3"/>
         <v>0.50652741514360311</v>
       </c>
-      <c r="I19" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L19">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -1279,10 +1239,6 @@
         <f t="shared" si="3"/>
         <v>0.87284287011807449</v>
       </c>
-      <c r="I20" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="L20">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -1316,7 +1272,14 @@
         <f>D21/F21</f>
         <v>0.84408152127820413</v>
       </c>
-      <c r="I21" s="13"/>
+      <c r="H21" s="12">
+        <f>SUM(H4:H20)</f>
+        <v>16100</v>
+      </c>
+      <c r="I21" s="13">
+        <f t="shared" ref="I21" si="8">H21/86400</f>
+        <v>0.18634259259259259</v>
+      </c>
       <c r="J21" s="11">
         <f>SUM(J4:J20)</f>
         <v>49447</v>
@@ -1364,7 +1327,7 @@
         <v>19670</v>
       </c>
       <c r="G24" s="5">
-        <f t="shared" ref="G24:G29" si="8">D24/F24</f>
+        <f t="shared" ref="G24:G29" si="9">D24/F24</f>
         <v>0.9718352821555668</v>
       </c>
       <c r="I24"/>
@@ -1391,7 +1354,7 @@
         <v>13875</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.74313513513513518</v>
       </c>
       <c r="I25"/>
@@ -1422,39 +1385,39 @@
         <v>41</v>
       </c>
       <c r="D28">
-        <v>403</v>
+        <v>420</v>
       </c>
       <c r="E28">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F29" si="9">D28+E28</f>
+        <f t="shared" ref="F28" si="10">D28+E28</f>
         <v>459</v>
       </c>
       <c r="G28" s="5">
-        <f t="shared" si="8"/>
-        <v>0.87799564270152508</v>
+        <f t="shared" si="9"/>
+        <v>0.91503267973856206</v>
       </c>
       <c r="H28">
-        <v>52</v>
-      </c>
-      <c r="I28">
+        <v>93</v>
+      </c>
+      <c r="I28" s="18">
         <f t="shared" si="4"/>
-        <v>6.018518518518519E-4</v>
+        <v>1.0763888888888889E-3</v>
       </c>
       <c r="J28">
-        <v>403</v>
+        <v>420</v>
       </c>
       <c r="K28">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="L28" s="3">
-        <f t="shared" ref="L28:L29" si="10">J28+K28</f>
+        <f t="shared" ref="L28:L29" si="11">J28+K28</f>
         <v>459</v>
       </c>
       <c r="M28" s="5">
-        <f t="shared" ref="M28:M29" si="11">J28/L28</f>
-        <v>0.87799564270152508</v>
+        <f t="shared" ref="M28:M29" si="12">J28/L28</f>
+        <v>0.91503267973856206</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1471,33 +1434,33 @@
         <v>419</v>
       </c>
       <c r="F29" s="3">
+        <f t="shared" ref="F29" si="13">D29+E29</f>
+        <v>4167</v>
+      </c>
+      <c r="G29" s="5">
         <f t="shared" si="9"/>
-        <v>4167</v>
-      </c>
-      <c r="G29" s="5">
-        <f t="shared" si="8"/>
         <v>0.89944804415646751</v>
       </c>
       <c r="H29">
-        <v>415</v>
-      </c>
-      <c r="I29">
+        <v>872</v>
+      </c>
+      <c r="I29" s="18">
         <f t="shared" si="4"/>
-        <v>4.8032407407407407E-3</v>
+        <v>1.0092592592592592E-2</v>
       </c>
       <c r="J29">
-        <v>3748</v>
+        <v>4366</v>
       </c>
       <c r="K29">
-        <v>419</v>
+        <v>349</v>
       </c>
       <c r="L29" s="3">
-        <f t="shared" si="10"/>
-        <v>4167</v>
+        <f t="shared" si="11"/>
+        <v>4715</v>
       </c>
       <c r="M29" s="5">
-        <f t="shared" si="11"/>
-        <v>0.89944804415646751</v>
+        <f t="shared" si="12"/>
+        <v>0.92598091198303289</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1529,21 +1492,41 @@
       <c r="I30" s="13"/>
       <c r="M30" s="14"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="G31"/>
+      <c r="I31"/>
+      <c r="J31">
+        <v>4242</v>
+      </c>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
         <f>9300*30000</f>
         <v>279000000</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
         <f>14000*14693</f>
         <v>205702000</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="3">
-        <f>B33-B34</f>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <f>B34-B35</f>
         <v>73298000</v>
       </c>
     </row>
@@ -1593,9 +1576,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1747,19 +1733,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1783,9 +1765,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update SERBER && STATS.xls
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -67,9 +67,6 @@
     <t>En nombre de jour et heures</t>
   </si>
   <si>
-    <t>RHOME EXPRESS COMMUNS</t>
-  </si>
-  <si>
     <t>Première passe en comparant station par station</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>SEMALY</t>
+  </si>
+  <si>
+    <t>RHONE EXPRESS COMMUNS</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,19 +609,19 @@
   <sheetData>
     <row r="1" spans="1:13" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="15"/>
       <c r="H2" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
@@ -638,16 +638,16 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>8</v>
@@ -656,16 +656,16 @@
         <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -693,8 +693,12 @@
         <f>D4/F4</f>
         <v>0.95217306567920479</v>
       </c>
+      <c r="I4" s="7">
+        <f t="shared" ref="I4:I30" si="2">H4/86400</f>
+        <v>0</v>
+      </c>
       <c r="L4">
-        <f t="shared" ref="L4:L14" si="2">J4+K4</f>
+        <f t="shared" ref="L4:L14" si="3">J4+K4</f>
         <v>0</v>
       </c>
     </row>
@@ -720,14 +724,14 @@
         <v>34459</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G20" si="3">D5/F5</f>
+        <f t="shared" ref="G5:G20" si="4">D5/F5</f>
         <v>0.86508604428451208</v>
       </c>
       <c r="H5">
         <v>13000</v>
       </c>
       <c r="I5" s="7">
-        <f t="shared" ref="I5:I30" si="4">H5/86400</f>
+        <f t="shared" si="2"/>
         <v>0.15046296296296297</v>
       </c>
       <c r="J5">
@@ -737,11 +741,11 @@
         <v>1293</v>
       </c>
       <c r="L5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34459</v>
       </c>
       <c r="M5" s="5">
-        <f t="shared" ref="M5:M6" si="5">J5/L5</f>
+        <f t="shared" ref="M5:M11" si="5">J5/L5</f>
         <v>0.96247714675411356</v>
       </c>
     </row>
@@ -767,14 +771,14 @@
         <v>8936</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.97996866606982991</v>
       </c>
       <c r="H6" s="10">
         <v>1500</v>
       </c>
       <c r="I6" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="J6">
@@ -784,7 +788,7 @@
         <v>176</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8940</v>
       </c>
       <c r="M6" s="5">
@@ -812,12 +816,20 @@
         <v>34932</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.92751631741669527</v>
       </c>
-      <c r="L7">
+      <c r="I7" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -845,9 +857,17 @@
         <f>D8/F8</f>
         <v>0.4597927658762952</v>
       </c>
-      <c r="L8">
+      <c r="I8" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -868,16 +888,33 @@
         <v>339</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f>D9+E9</f>
         <v>3409</v>
       </c>
       <c r="G9" s="5">
         <f>D9/F9</f>
         <v>0.9005573481959519</v>
       </c>
+      <c r="H9">
+        <v>168</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="2"/>
+        <v>1.9444444444444444E-3</v>
+      </c>
+      <c r="J9">
+        <v>3040</v>
+      </c>
+      <c r="K9">
+        <v>338</v>
+      </c>
       <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3378</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" si="5"/>
+        <v>0.89994079336885735</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -902,12 +939,20 @@
         <v>20512</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9863494539781591</v>
       </c>
-      <c r="L10">
+      <c r="I10" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -932,17 +977,25 @@
         <v>44</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.88636363636363635</v>
       </c>
-      <c r="L11">
+      <c r="I11" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="9">
         <v>500</v>
@@ -952,27 +1005,44 @@
         <v>5.7870370370370367E-3</v>
       </c>
       <c r="D12">
-        <v>4582</v>
+        <v>4612</v>
       </c>
       <c r="E12">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>4923</v>
+        <v>4973</v>
       </c>
       <c r="G12" s="5">
+        <f t="shared" si="4"/>
+        <v>0.92740800321737382</v>
+      </c>
+      <c r="H12">
+        <v>260</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="2"/>
+        <v>3.0092592592592593E-3</v>
+      </c>
+      <c r="J12">
+        <v>4675</v>
+      </c>
+      <c r="K12">
+        <v>301</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="3"/>
-        <v>0.93073329270769856</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4976</v>
+      </c>
+      <c r="M12" s="5">
+        <f>J12/L12</f>
+        <v>0.93950964630225076</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="9">
         <v>750</v>
@@ -992,12 +1062,29 @@
         <v>8052</v>
       </c>
       <c r="G13" s="5">
+        <f t="shared" si="4"/>
+        <v>0.9699453551912568</v>
+      </c>
+      <c r="H13">
+        <v>914</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0578703703703703E-2</v>
+      </c>
+      <c r="J13">
+        <v>7223</v>
+      </c>
+      <c r="K13">
+        <v>140</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="3"/>
-        <v>0.9699453551912568</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7363</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" ref="M13" si="6">J13/L13</f>
+        <v>0.98098601113676487</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1012,22 +1099,39 @@
         <v>1.4074074074074074E-2</v>
       </c>
       <c r="D14">
-        <v>10317</v>
+        <v>11000</v>
       </c>
       <c r="E14">
-        <v>738</v>
+        <v>802</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>11055</v>
+        <v>11802</v>
       </c>
       <c r="G14" s="5">
+        <f t="shared" si="4"/>
+        <v>0.93204541603118118</v>
+      </c>
+      <c r="H14">
+        <v>483</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="2"/>
+        <v>5.5902777777777773E-3</v>
+      </c>
+      <c r="J14">
+        <v>10134</v>
+      </c>
+      <c r="K14">
+        <v>674</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="3"/>
-        <v>0.93324287652645865</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10808</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" ref="M14:M15" si="7">J14/L14</f>
+        <v>0.93763878608438189</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1052,14 +1156,14 @@
         <v>6802</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.87915319023816529</v>
       </c>
       <c r="H15">
         <v>1451</v>
       </c>
       <c r="I15" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.6793981481481483E-2</v>
       </c>
       <c r="J15">
@@ -1073,7 +1177,7 @@
         <v>6804</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" ref="M15" si="6">J15/L15</f>
+        <f t="shared" si="7"/>
         <v>0.99382716049382713</v>
       </c>
     </row>
@@ -1099,14 +1203,14 @@
         <v>791</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.94690265486725667</v>
       </c>
       <c r="H16">
         <v>149</v>
       </c>
       <c r="I16" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.724537037037037E-3</v>
       </c>
       <c r="J16">
@@ -1116,7 +1220,7 @@
         <v>36</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L16:L20" si="7">J16+K16</f>
+        <f t="shared" ref="L16:L20" si="8">J16+K16</f>
         <v>791</v>
       </c>
       <c r="M16" s="5">
@@ -1146,11 +1250,11 @@
         <v>1217</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.98027937551355793</v>
       </c>
       <c r="L17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1176,17 +1280,17 @@
         <v>10036</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.76106018333997605</v>
       </c>
       <c r="L18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3">
         <v>21</v>
@@ -1206,11 +1310,11 @@
         <v>766</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.50652741514360311</v>
       </c>
       <c r="L19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1236,17 +1340,17 @@
         <v>1101</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.87284287011807449</v>
       </c>
       <c r="L20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="12">
         <f>SUM(B4:B20)</f>
@@ -1258,43 +1362,43 @@
       </c>
       <c r="D21" s="12">
         <f>SUM(D4:D20)</f>
-        <v>228909</v>
+        <v>229622</v>
       </c>
       <c r="E21" s="12">
         <f>SUM(E4:E20)</f>
-        <v>42284</v>
+        <v>42368</v>
       </c>
       <c r="F21" s="12">
         <f>SUM(F4:F20)</f>
-        <v>271193</v>
+        <v>271990</v>
       </c>
       <c r="G21" s="14">
         <f>D21/F21</f>
-        <v>0.84408152127820413</v>
+        <v>0.84422956726350229</v>
       </c>
       <c r="H21" s="12">
         <f>SUM(H4:H20)</f>
-        <v>16100</v>
+        <v>17925</v>
       </c>
       <c r="I21" s="13">
-        <f t="shared" ref="I21" si="8">H21/86400</f>
-        <v>0.18634259259259259</v>
+        <f t="shared" ref="I21" si="9">H21/86400</f>
+        <v>0.20746527777777779</v>
       </c>
       <c r="J21" s="11">
         <f>SUM(J4:J20)</f>
-        <v>49447</v>
+        <v>74519</v>
       </c>
       <c r="K21" s="11">
         <f>SUM(K4:K20)</f>
-        <v>1547</v>
+        <v>3000</v>
       </c>
       <c r="L21" s="11">
         <f>SUM(L4:L20)</f>
-        <v>50994</v>
+        <v>77519</v>
       </c>
       <c r="M21" s="14">
         <f>J21/L21</f>
-        <v>0.96966309761932779</v>
+        <v>0.96129981036907086</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1307,7 +1411,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="3">
         <v>877</v>
@@ -1327,14 +1431,14 @@
         <v>19670</v>
       </c>
       <c r="G24" s="5">
-        <f t="shared" ref="G24:G29" si="9">D24/F24</f>
+        <f t="shared" ref="G24:G29" si="10">D24/F24</f>
         <v>0.9718352821555668</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3">
         <v>995</v>
@@ -1354,14 +1458,14 @@
         <v>13875</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.74313513513513518</v>
       </c>
       <c r="I25"/>
     </row>
     <row r="26" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="13">
@@ -1379,7 +1483,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="3">
         <v>41</v>
@@ -1391,41 +1495,41 @@
         <v>39</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28" si="10">D28+E28</f>
+        <f t="shared" ref="F28" si="11">D28+E28</f>
         <v>459</v>
       </c>
       <c r="G28" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.91503267973856206</v>
       </c>
       <c r="H28">
         <v>93</v>
       </c>
       <c r="I28" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.0763888888888889E-3</v>
       </c>
       <c r="J28">
-        <v>420</v>
+        <v>453</v>
       </c>
       <c r="K28">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="L28" s="3">
-        <f t="shared" ref="L28:L29" si="11">J28+K28</f>
-        <v>459</v>
+        <f t="shared" ref="L28:L29" si="12">J28+K28</f>
+        <v>458</v>
       </c>
       <c r="M28" s="5">
-        <f t="shared" ref="M28:M29" si="12">J28/L28</f>
-        <v>0.91503267973856206</v>
+        <f t="shared" ref="M28:M29" si="13">J28/L28</f>
+        <v>0.98908296943231444</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D29">
         <v>3748</v>
@@ -1434,38 +1538,38 @@
         <v>419</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" ref="F29" si="13">D29+E29</f>
+        <f t="shared" ref="F29" si="14">D29+E29</f>
         <v>4167</v>
       </c>
       <c r="G29" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.89944804415646751</v>
       </c>
       <c r="H29">
         <v>872</v>
       </c>
       <c r="I29" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.0092592592592592E-2</v>
       </c>
       <c r="J29">
-        <v>4366</v>
+        <v>4329</v>
       </c>
       <c r="K29">
-        <v>349</v>
+        <v>38</v>
       </c>
       <c r="L29" s="3">
-        <f t="shared" si="11"/>
-        <v>4715</v>
+        <f t="shared" si="12"/>
+        <v>4367</v>
       </c>
       <c r="M29" s="5">
-        <f t="shared" si="12"/>
-        <v>0.92598091198303289</v>
+        <f t="shared" si="13"/>
+        <v>0.99129837416991073</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="12">
         <v>62000</v>
@@ -1497,19 +1601,16 @@
       <c r="C31"/>
       <c r="G31"/>
       <c r="I31"/>
-      <c r="J31">
-        <v>4242</v>
-      </c>
       <c r="M31"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,7 +1637,7 @@
     <mergeCell ref="H2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="percent" val="80"/>
         <cfvo type="percent" val="90"/>
@@ -1547,23 +1648,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M30:M1048576 M1:M27">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="percent" val="80"/>
-        <cfvo type="percent" val="90"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M28:M29">
+  <conditionalFormatting sqref="M1:M1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="percent" val="80"/>
         <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
         <cfvo type="percent" val="100"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>

</xml_diff>

<commit_message>
exclusion Archmac serber && script mr tram && stats
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -591,7 +591,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="J26" sqref="J26:M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1492,8 @@
         <v>0.88893120342541887</v>
       </c>
       <c r="I26" s="13"/>
-      <c r="M26" s="14"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F27" s="3"/>
@@ -1599,15 +1600,15 @@
         <v>23533</v>
       </c>
       <c r="E30" s="11">
-        <v>6707</v>
+        <v>1209</v>
       </c>
       <c r="F30" s="11">
         <f>D30+E30</f>
-        <v>30240</v>
+        <v>24742</v>
       </c>
       <c r="G30" s="14">
         <f>D30/F30</f>
-        <v>0.77820767195767193</v>
+        <v>0.9511357206369736</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="13"/>
@@ -1654,7 +1655,7 @@
     <mergeCell ref="H2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percent" val="80"/>
         <cfvo type="percent" val="90"/>
@@ -1665,11 +1666,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="M1:M25 M27:M1048576">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="percent" val="90"/>
         <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="percent" val="80"/>
+        <cfvo type="percent" val="90"/>
         <cfvo type="percent" val="100"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -1830,18 +1843,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1863,18 +1876,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
versionning SERBER && update STATS && extract with all Darfeuille
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t xml:space="preserve">LIGNE </t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>RHONE EXPRESS COMMUNS</t>
+  </si>
+  <si>
+    <t>FUNI COMMUNS + STATIONS</t>
+  </si>
+  <si>
+    <t>METRO ABCD INTERSTATIONS</t>
+  </si>
+  <si>
+    <t>METRO ABC,AB,A,B,C,D COMMUNS</t>
   </si>
 </sst>
 </file>
@@ -255,7 +264,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -264,7 +273,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -281,6 +289,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
@@ -589,15 +599,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="15" style="3" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" style="7" customWidth="1"/>
     <col min="4" max="6" width="13" customWidth="1"/>
@@ -612,21 +622,30 @@
       <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="G1" s="5">
+        <v>1</v>
+      </c>
       <c r="H1" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="M1" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="H2" s="17" t="s">
+      <c r="C2" s="15"/>
+      <c r="G2" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
       <c r="M2" s="5">
         <v>0.01</v>
       </c>
@@ -680,7 +699,7 @@
         <v>8289</v>
       </c>
       <c r="C4" s="7">
-        <f t="shared" ref="C4:C30" si="0">B4/86400</f>
+        <f t="shared" ref="C4:C33" si="0">B4/86400</f>
         <v>9.5937499999999995E-2</v>
       </c>
       <c r="D4">
@@ -690,20 +709,33 @@
         <v>3681</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F20" si="1">D4+E4</f>
+        <f t="shared" ref="F4:F22" si="1">D4+E4</f>
         <v>76965</v>
       </c>
       <c r="G4" s="5">
         <f>D4/F4</f>
         <v>0.95217306567920479</v>
       </c>
+      <c r="H4">
+        <v>1817</v>
+      </c>
       <c r="I4" s="7">
-        <f t="shared" ref="I4:I29" si="2">H4/86400</f>
-        <v>0</v>
+        <f t="shared" ref="I4:I32" si="2">H4/86400</f>
+        <v>2.1030092592592593E-2</v>
+      </c>
+      <c r="J4">
+        <v>69025</v>
+      </c>
+      <c r="K4">
+        <v>927</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L14" si="3">J4+K4</f>
-        <v>0</v>
+        <f t="shared" ref="L4:L16" si="3">J4+K4</f>
+        <v>69952</v>
+      </c>
+      <c r="M4" s="5">
+        <f t="shared" ref="M4:M10" si="4">J4/L4</f>
+        <v>0.98674805580969804</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -728,7 +760,7 @@
         <v>34459</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G20" si="4">D5/F5</f>
+        <f t="shared" ref="G5:G22" si="5">D5/F5</f>
         <v>0.86508604428451208</v>
       </c>
       <c r="H5">
@@ -749,7 +781,7 @@
         <v>34459</v>
       </c>
       <c r="M5" s="5">
-        <f t="shared" ref="M5:M11" si="5">J5/L5</f>
+        <f t="shared" si="4"/>
         <v>0.96247714675411356</v>
       </c>
     </row>
@@ -775,10 +807,10 @@
         <v>8936</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.97996866606982991</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6">
         <v>1500</v>
       </c>
       <c r="I6" s="7">
@@ -796,7 +828,7 @@
         <v>8940</v>
       </c>
       <c r="M6" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.98031319910514536</v>
       </c>
     </row>
@@ -804,10 +836,12 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7">
+        <v>4000</v>
+      </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.6296296296296294E-2</v>
       </c>
       <c r="D7">
         <v>32400</v>
@@ -820,20 +854,29 @@
         <v>34932</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.92751631741669527</v>
+      </c>
+      <c r="H7">
+        <v>4400</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.0925925925925923E-2</v>
+      </c>
+      <c r="J7">
+        <v>30377</v>
+      </c>
+      <c r="K7">
+        <v>2137</v>
       </c>
       <c r="L7">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>32514</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" si="4"/>
+        <v>0.93427446638371159</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -848,18 +891,18 @@
         <v>1.068287037037037E-2</v>
       </c>
       <c r="D8">
-        <v>21699</v>
+        <v>20430</v>
       </c>
       <c r="E8">
-        <v>25494</v>
+        <v>25490</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>47193</v>
+        <v>45920</v>
       </c>
       <c r="G8" s="5">
         <f>D8/F8</f>
-        <v>0.4597927658762952</v>
+        <v>0.44490418118466901</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="2"/>
@@ -870,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="5" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -917,7 +960,7 @@
         <v>3378</v>
       </c>
       <c r="M9" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.89994079336885735</v>
       </c>
     </row>
@@ -943,21 +986,15 @@
         <v>20512</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.9863494539781591</v>
       </c>
-      <c r="I10" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -981,350 +1018,345 @@
         <v>44</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.88636363636363635</v>
       </c>
-      <c r="I11" s="7">
+      <c r="H11" s="9"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="19"/>
+      <c r="H12">
+        <v>180</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="2"/>
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="J12">
+        <v>7261</v>
+      </c>
+      <c r="K12">
+        <v>159</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>7420</v>
+      </c>
+      <c r="M12" s="5">
+        <f>J12/L12</f>
+        <v>0.97857142857142854</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="19"/>
+      <c r="M13" s="5" t="e">
+        <f t="shared" ref="M13:M14" si="6">J13/L13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>500</v>
+      </c>
+      <c r="C14" s="7">
+        <f>B14/86400</f>
+        <v>5.7870370370370367E-3</v>
+      </c>
+      <c r="D14">
+        <v>4612</v>
+      </c>
+      <c r="E14">
+        <v>361</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>4973</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="5"/>
+        <v>0.92740800321737382</v>
+      </c>
+      <c r="H14">
+        <v>260</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="2"/>
+        <v>3.0092592592592593E-3</v>
+      </c>
+      <c r="J14">
+        <v>4675</v>
+      </c>
+      <c r="K14">
+        <v>301</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>4976</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="6"/>
+        <v>0.93950964630225076</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>750</v>
+      </c>
+      <c r="C15" s="7">
+        <f>B15/86400</f>
+        <v>8.6805555555555559E-3</v>
+      </c>
+      <c r="D15">
+        <v>7810</v>
+      </c>
+      <c r="E15">
+        <v>242</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>8052</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="5"/>
+        <v>0.9699453551912568</v>
+      </c>
+      <c r="H15">
+        <v>914</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0578703703703703E-2</v>
+      </c>
+      <c r="J15">
+        <v>7223</v>
+      </c>
+      <c r="K15">
+        <v>140</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>7363</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" ref="M15" si="7">J15/L15</f>
+        <v>0.98098601113676487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1216</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4074074074074074E-2</v>
+      </c>
+      <c r="D16">
+        <v>11000</v>
+      </c>
+      <c r="E16">
+        <v>802</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>11802</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="5"/>
+        <v>0.93204541603118118</v>
+      </c>
+      <c r="H16">
+        <v>483</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="2"/>
+        <v>5.5902777777777773E-3</v>
+      </c>
+      <c r="J16">
+        <v>10134</v>
+      </c>
+      <c r="K16">
+        <v>674</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>10808</v>
+      </c>
+      <c r="M16" s="5">
+        <f t="shared" ref="M16:M17" si="8">J16/L16</f>
+        <v>0.93763878608438189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3">
+        <v>224</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5925925925925925E-3</v>
+      </c>
+      <c r="D17">
+        <v>5980</v>
+      </c>
+      <c r="E17">
+        <v>822</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>6802</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="5"/>
+        <v>0.87915319023816529</v>
+      </c>
+      <c r="H17">
+        <v>1451</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="2"/>
+        <v>1.6793981481481483E-2</v>
+      </c>
+      <c r="J17">
+        <v>6762</v>
+      </c>
+      <c r="K17">
+        <v>42</v>
+      </c>
+      <c r="L17">
+        <f>J17+K17</f>
+        <v>6804</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" si="8"/>
+        <v>0.99382716049382713</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3">
+        <v>131</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5162037037037036E-3</v>
+      </c>
+      <c r="D18">
+        <v>749</v>
+      </c>
+      <c r="E18">
+        <v>42</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>791</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="5"/>
+        <v>0.94690265486725667</v>
+      </c>
+      <c r="H18">
+        <v>149</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="2"/>
+        <v>1.724537037037037E-3</v>
+      </c>
+      <c r="J18">
+        <v>755</v>
+      </c>
+      <c r="K18">
+        <v>36</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L23" si="9">J18+K18</f>
+        <v>791</v>
+      </c>
+      <c r="M18" s="5">
+        <f>J18/L18</f>
+        <v>0.95448798988621997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3">
+        <v>99</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="0"/>
+        <v>1.1458333333333333E-3</v>
+      </c>
+      <c r="D19">
+        <v>1193</v>
+      </c>
+      <c r="E19">
+        <v>24</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>1217</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="5"/>
+        <v>0.98027937551355793</v>
+      </c>
+      <c r="I19" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="9">
-        <v>500</v>
-      </c>
-      <c r="C12" s="7">
-        <f>B12/86400</f>
-        <v>5.7870370370370367E-3</v>
-      </c>
-      <c r="D12">
-        <v>4612</v>
-      </c>
-      <c r="E12">
-        <v>361</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>4973</v>
-      </c>
-      <c r="G12" s="5">
-        <f t="shared" si="4"/>
-        <v>0.92740800321737382</v>
-      </c>
-      <c r="H12">
-        <v>260</v>
-      </c>
-      <c r="I12" s="7">
-        <f t="shared" si="2"/>
-        <v>3.0092592592592593E-3</v>
-      </c>
-      <c r="J12">
-        <v>4675</v>
-      </c>
-      <c r="K12">
-        <v>301</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="3"/>
-        <v>4976</v>
-      </c>
-      <c r="M12" s="5">
-        <f>J12/L12</f>
-        <v>0.93950964630225076</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="9">
-        <v>750</v>
-      </c>
-      <c r="C13" s="7">
-        <f>B13/86400</f>
-        <v>8.6805555555555559E-3</v>
-      </c>
-      <c r="D13">
-        <v>7810</v>
-      </c>
-      <c r="E13">
-        <v>242</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>8052</v>
-      </c>
-      <c r="G13" s="5">
-        <f t="shared" si="4"/>
-        <v>0.9699453551912568</v>
-      </c>
-      <c r="H13">
-        <v>914</v>
-      </c>
-      <c r="I13" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0578703703703703E-2</v>
-      </c>
-      <c r="J13">
-        <v>7223</v>
-      </c>
-      <c r="K13">
-        <v>140</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
-        <v>7363</v>
-      </c>
-      <c r="M13" s="5">
-        <f t="shared" ref="M13" si="6">J13/L13</f>
-        <v>0.98098601113676487</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1216</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4074074074074074E-2</v>
-      </c>
-      <c r="D14">
-        <v>11000</v>
-      </c>
-      <c r="E14">
-        <v>802</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>11802</v>
-      </c>
-      <c r="G14" s="5">
-        <f t="shared" si="4"/>
-        <v>0.93204541603118118</v>
-      </c>
-      <c r="H14">
-        <v>483</v>
-      </c>
-      <c r="I14" s="7">
-        <f t="shared" si="2"/>
-        <v>5.5902777777777773E-3</v>
-      </c>
-      <c r="J14">
-        <v>10134</v>
-      </c>
-      <c r="K14">
-        <v>674</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="3"/>
-        <v>10808</v>
-      </c>
-      <c r="M14" s="5">
-        <f t="shared" ref="M14:M15" si="7">J14/L14</f>
-        <v>0.93763878608438189</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3">
-        <v>224</v>
-      </c>
-      <c r="C15" s="7">
-        <f t="shared" si="0"/>
-        <v>2.5925925925925925E-3</v>
-      </c>
-      <c r="D15">
-        <v>5980</v>
-      </c>
-      <c r="E15">
-        <v>822</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>6802</v>
-      </c>
-      <c r="G15" s="5">
-        <f t="shared" si="4"/>
-        <v>0.87915319023816529</v>
-      </c>
-      <c r="H15">
-        <v>1451</v>
-      </c>
-      <c r="I15" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6793981481481483E-2</v>
-      </c>
-      <c r="J15">
-        <v>6762</v>
-      </c>
-      <c r="K15">
-        <v>42</v>
-      </c>
-      <c r="L15">
-        <f>J15+K15</f>
-        <v>6804</v>
-      </c>
-      <c r="M15" s="5">
-        <f t="shared" si="7"/>
-        <v>0.99382716049382713</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3">
-        <v>131</v>
-      </c>
-      <c r="C16" s="7">
-        <f t="shared" si="0"/>
-        <v>1.5162037037037036E-3</v>
-      </c>
-      <c r="D16">
-        <v>749</v>
-      </c>
-      <c r="E16">
-        <v>42</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>791</v>
-      </c>
-      <c r="G16" s="5">
-        <f t="shared" si="4"/>
-        <v>0.94690265486725667</v>
-      </c>
-      <c r="H16">
-        <v>149</v>
-      </c>
-      <c r="I16" s="7">
-        <f t="shared" si="2"/>
-        <v>1.724537037037037E-3</v>
-      </c>
-      <c r="J16">
-        <v>755</v>
-      </c>
-      <c r="K16">
-        <v>36</v>
-      </c>
-      <c r="L16">
-        <f t="shared" ref="L16:L20" si="8">J16+K16</f>
-        <v>791</v>
-      </c>
-      <c r="M16" s="5">
-        <f>J16/L16</f>
-        <v>0.95448798988621997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="3">
-        <v>99</v>
-      </c>
-      <c r="C17" s="7">
-        <f t="shared" si="0"/>
-        <v>1.1458333333333333E-3</v>
-      </c>
-      <c r="D17">
-        <v>1193</v>
-      </c>
-      <c r="E17">
-        <v>24</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>1217</v>
-      </c>
-      <c r="G17" s="5">
-        <f t="shared" si="4"/>
-        <v>0.98027937551355793</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3">
-        <v>577</v>
-      </c>
-      <c r="C18" s="7">
-        <f t="shared" si="0"/>
-        <v>6.6782407407407407E-3</v>
-      </c>
-      <c r="D18">
-        <v>7638</v>
-      </c>
-      <c r="E18">
-        <v>2398</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="1"/>
-        <v>10036</v>
-      </c>
-      <c r="G18" s="5">
-        <f t="shared" si="4"/>
-        <v>0.76106018333997605</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="3">
-        <v>21</v>
-      </c>
-      <c r="C19" s="7">
-        <f t="shared" si="0"/>
-        <v>2.4305555555555555E-4</v>
-      </c>
-      <c r="D19">
-        <v>388</v>
-      </c>
-      <c r="E19">
-        <v>378</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
-        <v>766</v>
-      </c>
-      <c r="G19" s="5">
-        <f t="shared" si="4"/>
-        <v>0.50652741514360311</v>
+      <c r="J19">
+        <v>1143</v>
+      </c>
+      <c r="K19">
+        <v>23</v>
       </c>
       <c r="L19">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>1166</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" ref="M19:M23" si="10">J19/L19</f>
+        <v>0.98027444253859353</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3">
         <v>577</v>
@@ -1334,319 +1366,438 @@
         <v>6.6782407407407407E-3</v>
       </c>
       <c r="D20">
-        <v>961</v>
+        <v>7638</v>
       </c>
       <c r="E20">
-        <v>140</v>
+        <v>2398</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
+        <v>10036</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="5"/>
+        <v>0.76106018333997605</v>
+      </c>
+      <c r="H20">
+        <v>1994</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="2"/>
+        <v>2.3078703703703702E-2</v>
+      </c>
+      <c r="J20">
+        <v>6768</v>
+      </c>
+      <c r="K20">
+        <v>2179</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="9"/>
+        <v>8947</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" si="10"/>
+        <v>0.75645467754554596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3">
+        <v>21</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4305555555555555E-4</v>
+      </c>
+      <c r="D21">
+        <v>388</v>
+      </c>
+      <c r="E21">
+        <v>378</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>766</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="5"/>
+        <v>0.50652741514360311</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="5" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3">
+        <v>577</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="0"/>
+        <v>6.6782407407407407E-3</v>
+      </c>
+      <c r="D22">
+        <v>961</v>
+      </c>
+      <c r="E22">
+        <v>140</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
         <v>1101</v>
       </c>
-      <c r="G20" s="5">
-        <f t="shared" si="4"/>
+      <c r="G22" s="5">
+        <f t="shared" si="5"/>
         <v>0.87284287011807449</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="H22" s="9"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="19"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="19"/>
+      <c r="H23">
+        <v>300</v>
+      </c>
+      <c r="I23">
+        <f>H23/86400</f>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="J23">
+        <v>3054</v>
+      </c>
+      <c r="K23">
+        <v>115</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="9"/>
+        <v>3169</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="10"/>
+        <v>0.96371094982644367</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="12">
-        <f>SUM(B4:B20)</f>
-        <v>20686</v>
-      </c>
-      <c r="C21" s="13">
+      <c r="B24" s="11">
+        <f>SUM(B4:B22)</f>
+        <v>24686</v>
+      </c>
+      <c r="C24" s="12">
         <f t="shared" si="0"/>
-        <v>0.2394212962962963</v>
-      </c>
-      <c r="D21" s="12">
-        <f>SUM(D4:D20)</f>
-        <v>229622</v>
-      </c>
-      <c r="E21" s="12">
-        <f>SUM(E4:E20)</f>
-        <v>42368</v>
-      </c>
-      <c r="F21" s="12">
-        <f>SUM(F4:F20)</f>
-        <v>271990</v>
-      </c>
-      <c r="G21" s="14">
-        <f>D21/F21</f>
-        <v>0.84422956726350229</v>
-      </c>
-      <c r="H21" s="12">
-        <f>SUM(H4:H20)</f>
-        <v>17925</v>
-      </c>
-      <c r="I21" s="13">
-        <f t="shared" ref="I21" si="9">H21/86400</f>
-        <v>0.20746527777777779</v>
-      </c>
-      <c r="J21" s="11">
-        <f>SUM(J4:J20)</f>
-        <v>74519</v>
-      </c>
-      <c r="K21" s="11">
-        <f>SUM(K4:K20)</f>
-        <v>3000</v>
-      </c>
-      <c r="L21" s="11">
-        <f>SUM(L4:L20)</f>
-        <v>77519</v>
-      </c>
-      <c r="M21" s="14">
-        <f>J21/L21</f>
-        <v>0.96129981036907086</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F23" s="3"/>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+        <v>0.28571759259259261</v>
+      </c>
+      <c r="D24" s="11">
+        <f>SUM(D4:D22)</f>
+        <v>228353</v>
+      </c>
+      <c r="E24" s="11">
+        <f>SUM(E4:E22)</f>
+        <v>42364</v>
+      </c>
+      <c r="F24" s="11">
+        <f>SUM(F4:F22)</f>
+        <v>270717</v>
+      </c>
+      <c r="G24" s="13">
+        <f>D24/F24</f>
+        <v>0.84351185924784922</v>
+      </c>
+      <c r="H24" s="11">
+        <f>SUM(H4:H22)</f>
+        <v>26316</v>
+      </c>
+      <c r="I24" s="12">
+        <f>H24/86400</f>
+        <v>0.30458333333333332</v>
+      </c>
+      <c r="J24" s="10">
+        <f>SUM(J4:J23)</f>
+        <v>192147</v>
+      </c>
+      <c r="K24" s="10">
+        <f>SUM(K4:K23)</f>
+        <v>8540</v>
+      </c>
+      <c r="L24" s="10">
+        <f>SUM(L4:L22)</f>
+        <v>197518</v>
+      </c>
+      <c r="M24" s="13">
+        <f>J24/L24</f>
+        <v>0.97280754159114613</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B27" s="3">
         <v>877</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C27" s="7">
         <f t="shared" si="0"/>
         <v>1.0150462962962964E-2</v>
       </c>
-      <c r="D24">
+      <c r="D27">
         <v>19116</v>
       </c>
-      <c r="E24">
+      <c r="E27">
         <v>554</v>
       </c>
-      <c r="F24" s="3">
-        <f>D24+E24</f>
+      <c r="F27" s="3">
+        <f>D27+E27</f>
         <v>19670</v>
       </c>
-      <c r="G24" s="5">
-        <f t="shared" ref="G24:G29" si="10">D24/F24</f>
+      <c r="G27" s="5">
+        <f t="shared" ref="G27:G32" si="11">D27/F27</f>
         <v>0.9718352821555668</v>
       </c>
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B28" s="3">
         <v>995</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C28" s="7">
         <f t="shared" si="0"/>
         <v>1.1516203703703704E-2</v>
       </c>
-      <c r="D25">
+      <c r="D28">
         <v>10311</v>
       </c>
-      <c r="E25">
+      <c r="E28">
         <v>3564</v>
       </c>
-      <c r="F25" s="3">
-        <f>D25+E25</f>
+      <c r="F28" s="3">
+        <f>D28+E28</f>
         <v>13875</v>
       </c>
-      <c r="G25" s="5">
-        <f t="shared" si="10"/>
+      <c r="G28" s="5">
+        <f t="shared" si="11"/>
         <v>0.74313513513513518</v>
       </c>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B29" s="11">
         <v>25678</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C29" s="12">
         <f t="shared" si="0"/>
         <v>0.29719907407407409</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D29" s="10">
         <v>86365</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E29" s="10">
         <v>10791</v>
       </c>
-      <c r="F26" s="3">
-        <f>D26+E26</f>
+      <c r="F29" s="3">
+        <f>D29+E29</f>
         <v>97156</v>
       </c>
-      <c r="G26" s="5">
-        <f t="shared" si="10"/>
+      <c r="G29" s="5">
+        <f t="shared" si="11"/>
         <v>0.88893120342541887</v>
       </c>
-      <c r="I26" s="13"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F27" s="3"/>
-      <c r="I27"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="I29" s="12"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+      <c r="I30"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B31" s="3">
         <v>41</v>
       </c>
-      <c r="D28">
+      <c r="D31">
         <v>420</v>
       </c>
-      <c r="E28">
+      <c r="E31">
         <v>39</v>
       </c>
-      <c r="F28" s="3">
-        <f t="shared" ref="F28" si="11">D28+E28</f>
+      <c r="F31" s="3">
+        <f t="shared" ref="F31" si="12">D31+E31</f>
         <v>459</v>
       </c>
-      <c r="G28" s="5">
-        <f t="shared" si="10"/>
+      <c r="G31" s="5">
+        <f t="shared" si="11"/>
         <v>0.91503267973856206</v>
       </c>
-      <c r="H28">
+      <c r="H31">
         <v>93</v>
       </c>
-      <c r="I28" s="15">
+      <c r="I31" s="14">
         <f t="shared" si="2"/>
         <v>1.0763888888888889E-3</v>
       </c>
-      <c r="J28">
+      <c r="J31">
         <v>453</v>
       </c>
-      <c r="K28">
+      <c r="K31">
         <v>5</v>
       </c>
-      <c r="L28" s="3">
-        <f t="shared" ref="L28:L29" si="12">J28+K28</f>
+      <c r="L31" s="3">
+        <f t="shared" ref="L31:L32" si="13">J31+K31</f>
         <v>458</v>
       </c>
-      <c r="M28" s="5">
-        <f t="shared" ref="M28:M29" si="13">J28/L28</f>
+      <c r="M31" s="5">
+        <f t="shared" ref="M31:M32" si="14">J31/L31</f>
         <v>0.98908296943231444</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D29">
+      <c r="D32">
         <v>3748</v>
       </c>
-      <c r="E29">
+      <c r="E32">
         <v>419</v>
       </c>
-      <c r="F29" s="3">
-        <f t="shared" ref="F29" si="14">D29+E29</f>
+      <c r="F32" s="3">
+        <f t="shared" ref="F32" si="15">D32+E32</f>
         <v>4167</v>
       </c>
-      <c r="G29" s="5">
-        <f t="shared" si="10"/>
+      <c r="G32" s="5">
+        <f t="shared" si="11"/>
         <v>0.89944804415646751</v>
       </c>
-      <c r="H29">
-        <v>872</v>
-      </c>
-      <c r="I29" s="15">
+      <c r="H32">
+        <v>855</v>
+      </c>
+      <c r="I32" s="14">
         <f t="shared" si="2"/>
-        <v>1.0092592592592592E-2</v>
-      </c>
-      <c r="J29">
+        <v>9.8958333333333329E-3</v>
+      </c>
+      <c r="J32">
         <v>4329</v>
       </c>
-      <c r="K29">
+      <c r="K32">
         <v>38</v>
       </c>
-      <c r="L29" s="3">
-        <f t="shared" si="12"/>
+      <c r="L32" s="3">
+        <f t="shared" si="13"/>
         <v>4367</v>
       </c>
-      <c r="M29" s="5">
-        <f t="shared" si="13"/>
+      <c r="M32" s="5">
+        <f t="shared" si="14"/>
         <v>0.99129837416991073</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+    <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B33" s="11">
         <v>71386</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C33" s="12">
         <f t="shared" si="0"/>
         <v>0.82622685185185185</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D33" s="10">
         <v>23533</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E33" s="10">
         <v>1209</v>
       </c>
-      <c r="F30" s="11">
-        <f>D30+E30</f>
+      <c r="F33" s="10">
+        <f>D33+E33</f>
         <v>24742</v>
       </c>
-      <c r="G30" s="14">
-        <f>D30/F30</f>
+      <c r="G33" s="13">
+        <f>D33/F33</f>
         <v>0.9511357206369736</v>
       </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="13"/>
-      <c r="M30" s="14"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="G31"/>
-      <c r="I31"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="M33" s="13"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="G34"/>
+      <c r="I34"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
         <f>9300*30000</f>
         <v>279000000</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
         <f>14000*14693</f>
         <v>205702000</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="3">
-        <f>B34-B35</f>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <f>B37-B38</f>
         <v>73298000</v>
       </c>
     </row>
@@ -1667,7 +1818,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M25 M27:M1048576">
+  <conditionalFormatting sqref="M30:M1048576 M1:M28">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="percent" val="90"/>
@@ -1679,7 +1830,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
+  <conditionalFormatting sqref="M29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="80"/>

</xml_diff>

<commit_message>
add extract all darfeuille
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t xml:space="preserve">LIGNE </t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>METRO ABC,AB,A,B,C,D COMMUNS</t>
+  </si>
+  <si>
+    <t>3830?</t>
   </si>
 </sst>
 </file>
@@ -280,6 +283,8 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -289,8 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
@@ -602,7 +605,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,19 +636,19 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="17"/>
       <c r="G2" s="5">
         <v>0.01</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
       <c r="M2" s="5">
         <v>0.01</v>
       </c>
@@ -734,7 +737,7 @@
         <v>69952</v>
       </c>
       <c r="M4" s="5">
-        <f t="shared" ref="M4:M10" si="4">J4/L4</f>
+        <f t="shared" ref="M4:M9" si="4">J4/L4</f>
         <v>0.98674805580969804</v>
       </c>
     </row>
@@ -990,11 +993,11 @@
         <v>0.9863494539781591</v>
       </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="18"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="19"/>
+      <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1022,22 +1025,22 @@
         <v>0.88636363636363635</v>
       </c>
       <c r="H11" s="9"/>
-      <c r="I11" s="18"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="19"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="18"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="19"/>
+      <c r="G12" s="16"/>
       <c r="H12">
         <v>180</v>
       </c>
@@ -1065,14 +1068,31 @@
         <v>39</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="18"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="19"/>
-      <c r="M13" s="5" t="e">
+      <c r="G13" s="16"/>
+      <c r="H13">
+        <v>2856</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="2"/>
+        <v>3.3055555555555553E-2</v>
+      </c>
+      <c r="J13">
+        <v>39723</v>
+      </c>
+      <c r="K13">
+        <v>4626</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>44349</v>
+      </c>
+      <c r="M13" s="5">
         <f t="shared" ref="M13:M14" si="6">J13/L13</f>
-        <v>#DIV/0!</v>
+        <v>0.89569099641480077</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1426,9 +1446,12 @@
         <f t="shared" si="5"/>
         <v>0.50652741514360311</v>
       </c>
-      <c r="I21" s="7">
+      <c r="H21" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="7" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L21">
         <f t="shared" si="9"/>
@@ -1465,27 +1488,27 @@
         <v>0.87284287011807449</v>
       </c>
       <c r="H22" s="9"/>
-      <c r="I22" s="18"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
-      <c r="M22" s="19"/>
+      <c r="M22" s="16"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="18"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="19"/>
+      <c r="G23" s="16"/>
       <c r="H23">
         <v>300</v>
       </c>
-      <c r="I23">
-        <f>H23/86400</f>
+      <c r="I23" s="7">
+        <f t="shared" si="2"/>
         <v>3.472222222222222E-3</v>
       </c>
       <c r="J23">
@@ -1533,27 +1556,27 @@
       </c>
       <c r="H24" s="11">
         <f>SUM(H4:H22)</f>
-        <v>26316</v>
+        <v>29172</v>
       </c>
       <c r="I24" s="12">
         <f>H24/86400</f>
-        <v>0.30458333333333332</v>
+        <v>0.33763888888888888</v>
       </c>
       <c r="J24" s="10">
         <f>SUM(J4:J23)</f>
-        <v>192147</v>
+        <v>231870</v>
       </c>
       <c r="K24" s="10">
         <f>SUM(K4:K23)</f>
-        <v>8540</v>
+        <v>13166</v>
       </c>
       <c r="L24" s="10">
         <f>SUM(L4:L22)</f>
-        <v>197518</v>
+        <v>241867</v>
       </c>
       <c r="M24" s="13">
         <f>J24/L24</f>
-        <v>0.97280754159114613</v>
+        <v>0.95866736677595543</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1644,8 +1667,6 @@
         <v>0.88893120342541887</v>
       </c>
       <c r="I29" s="12"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F30" s="3"/>
@@ -1830,29 +1851,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M29">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="percent" val="80"/>
-        <cfvo type="percent" val="90"/>
-        <cfvo type="percent" val="100"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004955207F9F5B314B8B9B51B8E365D485" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c516aae3580213d3db2e32983502eaaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c1ef9b3-4174-4af3-a5b1-5f98b740a774" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c89a2e4264c97434fad65ccc84a3a390" ns2:_="">
     <xsd:import namespace="4c1ef9b3-4174-4af3-a5b1-5f98b740a774"/>
@@ -2000,6 +2003,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2010,15 +2019,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE5D3DB7-DCDC-44A8-A58C-499D0DB8587A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2036,6 +2036,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
new comparaison with Jaro-Winkler algo
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t xml:space="preserve">LIGNE </t>
   </si>
@@ -151,7 +151,10 @@
     <t xml:space="preserve">Traitement des 2 passes et passages des erreurs face à toute l'extraction </t>
   </si>
   <si>
-    <t>Tester surface avec agence bellecour et commun bus</t>
+    <t>Surface vs surface 3h43 pour 20498 succès et 42518 échecs,  après reprise des échecs sur tout hors ligne fortes :</t>
+  </si>
+  <si>
+    <t>En comparant les échecs à tout darfeuille on passe de 14842 échecs à 11388</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,18 +872,18 @@
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="J6" s="17">
-        <v>8764</v>
+        <v>7802</v>
       </c>
       <c r="K6" s="17">
-        <v>176</v>
+        <v>4</v>
       </c>
       <c r="L6" s="17">
         <f t="shared" si="3"/>
-        <v>8940</v>
+        <v>7806</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="4"/>
-        <v>0.98031319910514536</v>
+        <v>0.99948757366128615</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1262,18 +1265,18 @@
         <v>1.724537037037037E-3</v>
       </c>
       <c r="J15" s="17">
-        <v>755</v>
+        <v>776</v>
       </c>
       <c r="K15" s="17">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="L15" s="17">
         <f t="shared" ref="L15:L23" si="9">J15+K15</f>
-        <v>791</v>
+        <v>779</v>
       </c>
       <c r="M15" s="5">
         <f>J15/L15</f>
-        <v>0.95448798988621997</v>
+        <v>0.99614890885750962</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1324,32 +1327,35 @@
       <c r="A17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="16"/>
+      <c r="B17" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
       <c r="H17">
-        <v>9000</v>
+        <v>100666</v>
       </c>
       <c r="I17" s="22">
         <f t="shared" si="2"/>
-        <v>0.10416666666666667</v>
+        <v>1.1651157407407406</v>
       </c>
       <c r="J17" s="17">
-        <v>42780</v>
+        <f>42780+3456</f>
+        <v>46236</v>
       </c>
       <c r="K17" s="20">
-        <v>14842</v>
+        <v>11388</v>
       </c>
       <c r="L17" s="17">
         <f t="shared" si="9"/>
-        <v>57622</v>
+        <v>57624</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" si="10"/>
-        <v>0.74242476831765647</v>
+        <v>0.80237401082882132</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1385,18 +1391,18 @@
         <v>2.3078703703703702E-2</v>
       </c>
       <c r="J18" s="17">
-        <v>6768</v>
+        <v>6565</v>
       </c>
       <c r="K18" s="20">
-        <v>2179</v>
+        <v>30</v>
       </c>
       <c r="L18" s="17">
         <f t="shared" si="9"/>
-        <v>8947</v>
+        <v>6595</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="10"/>
-        <v>0.75645467754554596</v>
+        <v>0.99545109931766484</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1523,25 +1529,25 @@
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22">
-        <v>13427</v>
+        <v>106666</v>
       </c>
       <c r="I22" s="22">
         <f t="shared" si="2"/>
-        <v>0.15540509259259258</v>
+        <v>1.2345601851851853</v>
       </c>
       <c r="J22" s="17">
-        <v>20498</v>
+        <v>38256</v>
       </c>
       <c r="K22" s="20">
-        <v>42518</v>
+        <v>24660</v>
       </c>
       <c r="L22" s="17">
         <f t="shared" si="9"/>
-        <v>63016</v>
+        <v>62916</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="10"/>
-        <v>0.32528246794464899</v>
+        <v>0.60804882700743845</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1605,28 +1611,28 @@
         <v>0.83065405799284353</v>
       </c>
       <c r="H24" s="11">
-        <f>SUM(H4:H19)</f>
-        <v>66123</v>
+        <f>SUM(H4:H23)</f>
+        <v>265045</v>
       </c>
       <c r="I24" s="21">
         <f t="shared" si="2"/>
-        <v>0.76531249999999995</v>
+        <v>3.0676504629629631</v>
       </c>
       <c r="J24" s="19">
         <f>SUM(J4:J23)</f>
-        <v>329292</v>
+        <v>349362</v>
       </c>
       <c r="K24" s="19">
         <f>SUM(K4:K23)</f>
-        <v>91767</v>
+        <v>68101</v>
       </c>
       <c r="L24" s="19">
         <f>SUM(L4:L23)</f>
-        <v>421059</v>
+        <v>417463</v>
       </c>
       <c r="M24" s="13">
         <f>J24/L24</f>
-        <v>0.78205667139284518</v>
+        <v>0.83686937525002214</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1649,11 +1655,11 @@
       <c r="K25" s="27"/>
       <c r="L25" s="17">
         <f>414217-L24</f>
-        <v>-6842</v>
+        <v>-3246</v>
       </c>
       <c r="M25" s="5">
         <f>1-L25/414217</f>
-        <v>1.0165179121088705</v>
+        <v>1.0078364721872834</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1673,11 +1679,11 @@
       <c r="G27" s="28"/>
       <c r="H27" s="17">
         <f>K24*5</f>
-        <v>458835</v>
+        <v>340505</v>
       </c>
       <c r="I27" s="22">
         <f>(H27/86400)+I24</f>
-        <v>6.0759027777777783</v>
+        <v>7.0086805555555554</v>
       </c>
       <c r="K27" s="7"/>
     </row>
@@ -1927,15 +1933,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="I25:K25"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B17:G17"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:G21 G26 G28:G1048576 G23:G24">
+  <conditionalFormatting sqref="G1:G16 G26 G28:G1048576 G23:G24 G18:G21">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percent" val="80"/>
@@ -1965,21 +1972,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004955207F9F5B314B8B9B51B8E365D485" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c516aae3580213d3db2e32983502eaaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c1ef9b3-4174-4af3-a5b1-5f98b740a774" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c89a2e4264c97434fad65ccc84a3a390" ns2:_="">
     <xsd:import namespace="4c1ef9b3-4174-4af3-a5b1-5f98b740a774"/>
@@ -2127,15 +2125,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2144,7 +2143,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE5D3DB7-DCDC-44A8-A58C-499D0DB8587A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2160,4 +2159,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
modify start timeit && remove few print
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -656,7 +656,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,6 +1978,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004955207F9F5B314B8B9B51B8E365D485" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c516aae3580213d3db2e32983502eaaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c1ef9b3-4174-4af3-a5b1-5f98b740a774" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c89a2e4264c97434fad65ccc84a3a390" ns2:_="">
     <xsd:import namespace="4c1ef9b3-4174-4af3-a5b1-5f98b740a774"/>
@@ -2125,15 +2134,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
   <ds:schemaRefs>
@@ -2144,6 +2144,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE5D3DB7-DCDC-44A8-A58C-499D0DB8587A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2159,12 +2167,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
delete few print && clean code
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -656,7 +656,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,18 +1502,18 @@
         <v>2.0370370370370369E-3</v>
       </c>
       <c r="J21" s="17">
-        <v>11674</v>
+        <v>11661</v>
       </c>
       <c r="K21" s="17">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L21" s="17">
         <f t="shared" si="9"/>
-        <v>11698</v>
+        <v>11683</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="10"/>
-        <v>0.99794836724226366</v>
+        <v>0.99811692202345292</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1620,19 +1620,19 @@
       </c>
       <c r="J24" s="19">
         <f>SUM(J4:J23)</f>
-        <v>346535</v>
+        <v>346522</v>
       </c>
       <c r="K24" s="19">
         <f>SUM(K4:K23)</f>
-        <v>67402</v>
+        <v>67400</v>
       </c>
       <c r="L24" s="19">
         <f>SUM(L4:L23)</f>
-        <v>413937</v>
+        <v>413922</v>
       </c>
       <c r="M24" s="13">
         <f>J24/L24</f>
-        <v>0.83716845800206308</v>
+        <v>0.83716738902498533</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1655,11 +1655,11 @@
       <c r="K25" s="27"/>
       <c r="L25" s="17">
         <f>414217-L24</f>
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="M25" s="5">
         <f>1-L25/414217</f>
-        <v>0.99932402581255719</v>
+        <v>0.99928781290965851</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1679,11 +1679,11 @@
       <c r="G27" s="28"/>
       <c r="H27" s="17">
         <f>K24*5</f>
-        <v>337010</v>
+        <v>337000</v>
       </c>
       <c r="I27" s="22">
         <f>(H27/86400)+I24</f>
-        <v>6.9682291666666671</v>
+        <v>6.9681134259259263</v>
       </c>
       <c r="K27" s="7"/>
     </row>
@@ -1972,6 +1972,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004955207F9F5B314B8B9B51B8E365D485" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c516aae3580213d3db2e32983502eaaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c1ef9b3-4174-4af3-a5b1-5f98b740a774" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c89a2e4264c97434fad65ccc84a3a390" ns2:_="">
     <xsd:import namespace="4c1ef9b3-4174-4af3-a5b1-5f98b740a774"/>
@@ -2119,22 +2134,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE5D3DB7-DCDC-44A8-A58C-499D0DB8587A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2150,21 +2167,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
value_only_tree_number && uptdate STATS
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t xml:space="preserve">LIGNE </t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>En comparant les échecs à tout darfeuille on passe de 14842 échecs à 11388</t>
+  </si>
+  <si>
+    <t>Analyse Dernière semaine</t>
+  </si>
+  <si>
+    <t>Il faut 4 jours pour faire la comparaison classique station sur station et ligne par ligne</t>
   </si>
 </sst>
 </file>
@@ -299,7 +305,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -323,6 +329,9 @@
     <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -344,6 +353,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
@@ -653,10 +663,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,9 +681,10 @@
     <col min="9" max="9" width="31.7109375" style="7" customWidth="1"/>
     <col min="10" max="12" width="14.28515625" style="17" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
@@ -685,26 +697,35 @@
       <c r="M1" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="24"/>
       <c r="G2" s="5">
         <v>0.01</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
       <c r="M2" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,8 +765,26 @@
       <c r="M3" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -788,11 +827,25 @@
         <v>66860</v>
       </c>
       <c r="M4" s="5">
-        <f t="shared" ref="M4:M8" si="4">J4/L4</f>
+        <f>J4/L4</f>
         <v>0.99913251570445705</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>66528</v>
+      </c>
+      <c r="Q4">
+        <v>2592</v>
+      </c>
+      <c r="R4" s="17">
+        <f>P4+Q4</f>
+        <v>69120</v>
+      </c>
+      <c r="S4" s="5">
+        <f>P4/R4</f>
+        <v>0.96250000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -814,7 +867,7 @@
         <v>34459</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G19" si="5">D5/F5</f>
+        <f t="shared" ref="G5:G19" si="4">D5/F5</f>
         <v>0.86508604428451208</v>
       </c>
       <c r="H5">
@@ -835,11 +888,25 @@
         <v>34459</v>
       </c>
       <c r="M5" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="M5:M8" si="5">J5/L5</f>
         <v>0.96247714675411356</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>29913</v>
+      </c>
+      <c r="Q5">
+        <v>2015</v>
+      </c>
+      <c r="R5" s="17">
+        <f t="shared" ref="R5:R23" si="6">P5+Q5</f>
+        <v>31928</v>
+      </c>
+      <c r="S5" s="5">
+        <f t="shared" ref="S5:S23" si="7">P5/R5</f>
+        <v>0.93688925081433228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -861,7 +928,7 @@
         <v>8936</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.97996866606982991</v>
       </c>
       <c r="H6">
@@ -882,11 +949,25 @@
         <v>7372</v>
       </c>
       <c r="M6" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.97639717851329355</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>6997</v>
+      </c>
+      <c r="Q6">
+        <v>297</v>
+      </c>
+      <c r="R6" s="17">
+        <f t="shared" si="6"/>
+        <v>7294</v>
+      </c>
+      <c r="S6" s="5">
+        <f t="shared" si="7"/>
+        <v>0.95928160131615026</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -908,7 +989,7 @@
         <v>34932</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.92751631741669527</v>
       </c>
       <c r="H7">
@@ -929,11 +1010,25 @@
         <v>32514</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.93427446638371159</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>27056</v>
+      </c>
+      <c r="Q7">
+        <v>2606</v>
+      </c>
+      <c r="R7" s="17">
+        <f t="shared" si="6"/>
+        <v>29662</v>
+      </c>
+      <c r="S7" s="5">
+        <f t="shared" si="7"/>
+        <v>0.9121434832445553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -976,11 +1071,25 @@
         <v>45932</v>
       </c>
       <c r="M8" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53644517983105455</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>20390</v>
+      </c>
+      <c r="Q8">
+        <v>25514</v>
+      </c>
+      <c r="R8" s="17">
+        <f t="shared" si="6"/>
+        <v>45904</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" si="7"/>
+        <v>0.44418787033809692</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1011,8 +1120,13 @@
         <f>J9/L9</f>
         <v>0.97857142857142854</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R9" s="17"/>
+      <c r="S9" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1040,11 +1154,25 @@
         <v>44349</v>
       </c>
       <c r="M10" s="5">
-        <f t="shared" ref="M10:M11" si="6">J10/L10</f>
+        <f t="shared" ref="M10:M11" si="8">J10/L10</f>
         <v>0.89569099641480077</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>39312</v>
+      </c>
+      <c r="Q10">
+        <v>4110</v>
+      </c>
+      <c r="R10" s="17">
+        <f t="shared" si="6"/>
+        <v>43422</v>
+      </c>
+      <c r="S10" s="5">
+        <f t="shared" si="7"/>
+        <v>0.90534751969047944</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1066,7 +1194,7 @@
         <v>4973</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.92740800321737382</v>
       </c>
       <c r="H11">
@@ -1087,11 +1215,25 @@
         <v>4976</v>
       </c>
       <c r="M11" s="5">
+        <f t="shared" si="8"/>
+        <v>0.93950964630225076</v>
+      </c>
+      <c r="P11">
+        <v>4610</v>
+      </c>
+      <c r="Q11">
+        <v>56</v>
+      </c>
+      <c r="R11" s="17">
         <f t="shared" si="6"/>
-        <v>0.93950964630225076</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4666</v>
+      </c>
+      <c r="S11" s="5">
+        <f t="shared" si="7"/>
+        <v>0.98799828546935275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1113,7 +1255,7 @@
         <v>8052</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.9699453551912568</v>
       </c>
       <c r="H12">
@@ -1134,11 +1276,25 @@
         <v>7363</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" ref="M12" si="7">J12/L12</f>
+        <f t="shared" ref="M12" si="9">J12/L12</f>
         <v>0.98098601113676487</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>7123</v>
+      </c>
+      <c r="Q12">
+        <v>95</v>
+      </c>
+      <c r="R12" s="17">
+        <f t="shared" si="6"/>
+        <v>7218</v>
+      </c>
+      <c r="S12" s="5">
+        <f t="shared" si="7"/>
+        <v>0.98683845940703796</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1160,7 +1316,7 @@
         <v>11802</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.93204541603118118</v>
       </c>
       <c r="H13">
@@ -1181,11 +1337,25 @@
         <v>10808</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" ref="M13:M14" si="8">J13/L13</f>
+        <f t="shared" ref="M13:M14" si="10">J13/L13</f>
         <v>0.93763878608438189</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>10070</v>
+      </c>
+      <c r="Q13">
+        <v>385</v>
+      </c>
+      <c r="R13" s="17">
+        <f t="shared" si="6"/>
+        <v>10455</v>
+      </c>
+      <c r="S13" s="5">
+        <f t="shared" si="7"/>
+        <v>0.96317551410808222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1207,7 +1377,7 @@
         <v>6802</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.87915319023816529</v>
       </c>
       <c r="H14">
@@ -1228,11 +1398,25 @@
         <v>6804</v>
       </c>
       <c r="M14" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99382716049382713</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>6395</v>
+      </c>
+      <c r="Q14">
+        <v>22</v>
+      </c>
+      <c r="R14" s="17">
+        <f t="shared" si="6"/>
+        <v>6417</v>
+      </c>
+      <c r="S14" s="5">
+        <f t="shared" si="7"/>
+        <v>0.99657160666978339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1254,7 +1438,7 @@
         <v>791</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.94690265486725667</v>
       </c>
       <c r="H15">
@@ -1271,15 +1455,29 @@
         <v>3</v>
       </c>
       <c r="L15" s="17">
-        <f t="shared" ref="L15:L23" si="9">J15+K15</f>
+        <f t="shared" ref="L15:L23" si="11">J15+K15</f>
         <v>779</v>
       </c>
       <c r="M15" s="5">
         <f>J15/L15</f>
         <v>0.99614890885750962</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>779</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15" s="17">
+        <f t="shared" si="6"/>
+        <v>782</v>
+      </c>
+      <c r="S15" s="5">
+        <f t="shared" si="7"/>
+        <v>0.99616368286445012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1301,7 +1499,7 @@
         <v>1217</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.98027937551355793</v>
       </c>
       <c r="I16" s="22">
@@ -1315,26 +1513,40 @@
         <v>23</v>
       </c>
       <c r="L16" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1166</v>
       </c>
       <c r="M16" s="5">
-        <f t="shared" ref="M16:M23" si="10">J16/L16</f>
+        <f t="shared" ref="M16:M23" si="12">J16/L16</f>
         <v>0.98027444253859353</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>1142</v>
+      </c>
+      <c r="Q16">
+        <v>21</v>
+      </c>
+      <c r="R16" s="17">
+        <f t="shared" si="6"/>
+        <v>1163</v>
+      </c>
+      <c r="S16" s="5">
+        <f t="shared" si="7"/>
+        <v>0.98194325021496132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
       <c r="H17">
         <v>100666</v>
       </c>
@@ -1350,15 +1562,29 @@
         <v>11388</v>
       </c>
       <c r="L17" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>57624</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.80237401082882132</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>43356</v>
+      </c>
+      <c r="Q17">
+        <v>13482</v>
+      </c>
+      <c r="R17" s="17">
+        <f t="shared" si="6"/>
+        <v>56838</v>
+      </c>
+      <c r="S17" s="5">
+        <f t="shared" si="7"/>
+        <v>0.76279953552200996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1380,7 +1606,7 @@
         <v>10036</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76106018333997605</v>
       </c>
       <c r="H18">
@@ -1397,15 +1623,29 @@
         <v>30</v>
       </c>
       <c r="L18" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6595</v>
       </c>
       <c r="M18" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.99545109931766484</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>6763</v>
+      </c>
+      <c r="Q18">
+        <v>1616</v>
+      </c>
+      <c r="R18" s="17">
+        <f t="shared" si="6"/>
+        <v>8379</v>
+      </c>
+      <c r="S18" s="5">
+        <f t="shared" si="7"/>
+        <v>0.80713688984365672</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1427,7 +1667,7 @@
         <v>766</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.50652741514360311</v>
       </c>
       <c r="H19">
@@ -1444,15 +1684,29 @@
         <v>248</v>
       </c>
       <c r="L19" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>764</v>
       </c>
       <c r="M19" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.67539267015706805</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>303</v>
+      </c>
+      <c r="Q19">
+        <v>377</v>
+      </c>
+      <c r="R19" s="17">
+        <f t="shared" si="6"/>
+        <v>680</v>
+      </c>
+      <c r="S19" s="5">
+        <f t="shared" si="7"/>
+        <v>0.44558823529411767</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1476,15 +1730,29 @@
         <v>115</v>
       </c>
       <c r="L20" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3169</v>
       </c>
       <c r="M20" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.96371094982644367</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>3027</v>
+      </c>
+      <c r="Q20">
+        <v>102</v>
+      </c>
+      <c r="R20" s="17">
+        <f t="shared" si="6"/>
+        <v>3129</v>
+      </c>
+      <c r="S20" s="5">
+        <f t="shared" si="7"/>
+        <v>0.96740172579098749</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1508,26 +1776,40 @@
         <v>22</v>
       </c>
       <c r="L21" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>11683</v>
       </c>
       <c r="M21" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.99811692202345292</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>11661</v>
+      </c>
+      <c r="Q21">
+        <v>22</v>
+      </c>
+      <c r="R21" s="17">
+        <f t="shared" si="6"/>
+        <v>11683</v>
+      </c>
+      <c r="S21" s="5">
+        <f t="shared" si="7"/>
+        <v>0.99811692202345292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
       <c r="H22">
         <v>106666</v>
       </c>
@@ -1542,15 +1824,29 @@
         <v>24660</v>
       </c>
       <c r="L22" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>62916</v>
       </c>
       <c r="M22" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.60804882700743845</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>38110</v>
+      </c>
+      <c r="Q22">
+        <v>24195</v>
+      </c>
+      <c r="R22" s="17">
+        <f t="shared" si="6"/>
+        <v>62305</v>
+      </c>
+      <c r="S22" s="5">
+        <f t="shared" si="7"/>
+        <v>0.61166840542492573</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1574,15 +1870,29 @@
         <v>15</v>
       </c>
       <c r="L23" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>369</v>
       </c>
       <c r="M23" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.95934959349593496</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>338</v>
+      </c>
+      <c r="Q23">
+        <v>32</v>
+      </c>
+      <c r="R23" s="17">
+        <f t="shared" si="6"/>
+        <v>370</v>
+      </c>
+      <c r="S23" s="5">
+        <f t="shared" si="7"/>
+        <v>0.91351351351351351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>19</v>
       </c>
@@ -1634,25 +1944,41 @@
         <f>J24/L24</f>
         <v>0.83716738902498533</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="19">
+        <f>SUM(P4:P23)</f>
+        <v>323873</v>
+      </c>
+      <c r="Q24" s="19">
+        <f>SUM(Q4:Q23)</f>
+        <v>77542</v>
+      </c>
+      <c r="R24" s="19">
+        <f>SUM(R4:R23)</f>
+        <v>401415</v>
+      </c>
+      <c r="S24" s="13">
+        <f>P24/R24</f>
+        <v>0.80682834473051579</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="17"/>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
       <c r="L25" s="17">
         <f>414217-L24</f>
         <v>295</v>
@@ -1661,22 +1987,29 @@
         <f>1-L25/414217</f>
         <v>0.99928781290965851</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <f>(Q24*5)/3600</f>
+        <v>107.69722222222222</v>
+      </c>
+      <c r="R25" s="17">
+        <v>414217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F26" s="3"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="17">
         <f>K24*5</f>
         <v>337000</v>
@@ -1686,12 +2019,26 @@
         <v>6.9681134259259263</v>
       </c>
       <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23" t="str">
+        <f>CONCATENATE("Il faut ",Q25," heures de plus pour faire la comparaison des erreurs sur darfeuille")</f>
+        <v>Il faut 107,697222222222 heures de plus pour faire la comparaison des erreurs sur darfeuille</v>
+      </c>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="31" t="str">
+        <f>CONCATENATE("Soit ",((Q25/24)+4)," jours")</f>
+        <v>Soit 8,48738425925926 jours</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
       <c r="I28"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S28"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1713,12 +2060,26 @@
         <v>19670</v>
       </c>
       <c r="G29" s="5">
-        <f t="shared" ref="G29:G34" si="11">D29/F29</f>
+        <f t="shared" ref="G29:G34" si="13">D29/F29</f>
         <v>0.9718352821555668</v>
       </c>
       <c r="I29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>7232</v>
+      </c>
+      <c r="Q29">
+        <v>378</v>
+      </c>
+      <c r="R29">
+        <f>P29+Q29</f>
+        <v>7610</v>
+      </c>
+      <c r="S29" s="13">
+        <f t="shared" ref="S29" si="14">P29/R29</f>
+        <v>0.95032851511169514</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1740,12 +2101,13 @@
         <v>13875</v>
       </c>
       <c r="G30" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.74313513513513518</v>
       </c>
       <c r="I30"/>
-    </row>
-    <row r="31" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S30"/>
+    </row>
+    <row r="31" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>25</v>
       </c>
@@ -1767,19 +2129,33 @@
         <v>97156</v>
       </c>
       <c r="G31" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.88893120342541887</v>
       </c>
       <c r="I31" s="12"/>
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P31" s="10">
+        <v>68040</v>
+      </c>
+      <c r="Q31" s="10">
+        <v>10562</v>
+      </c>
+      <c r="R31" s="10">
+        <f>P31+Q31</f>
+        <v>78602</v>
+      </c>
+      <c r="S31" s="13">
+        <f>P31/R31</f>
+        <v>0.86562682883387188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F32" s="3"/>
       <c r="I32"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1793,11 +2169,11 @@
         <v>39</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" ref="F33" si="12">D33+E33</f>
+        <f t="shared" ref="F33" si="15">D33+E33</f>
         <v>459</v>
       </c>
       <c r="G33" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.91503267973856206</v>
       </c>
       <c r="H33">
@@ -1814,15 +2190,15 @@
         <v>5</v>
       </c>
       <c r="L33" s="17">
-        <f t="shared" ref="L33:L34" si="13">J33+K33</f>
+        <f t="shared" ref="L33:L34" si="16">J33+K33</f>
         <v>458</v>
       </c>
       <c r="M33" s="5">
-        <f t="shared" ref="M33:M34" si="14">J33/L33</f>
+        <f t="shared" ref="M33:M34" si="17">J33/L33</f>
         <v>0.98908296943231444</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1836,11 +2212,11 @@
         <v>419</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" ref="F34" si="15">D34+E34</f>
+        <f t="shared" ref="F34" si="18">D34+E34</f>
         <v>4167</v>
       </c>
       <c r="G34" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.89944804415646751</v>
       </c>
       <c r="H34">
@@ -1857,15 +2233,15 @@
         <v>38</v>
       </c>
       <c r="L34" s="17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>4367</v>
       </c>
       <c r="M34" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.99129837416991073</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>26</v>
       </c>
@@ -1896,44 +2272,60 @@
       <c r="K35" s="19"/>
       <c r="L35" s="19"/>
       <c r="M35" s="13"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P35" s="10">
+        <v>23383</v>
+      </c>
+      <c r="Q35" s="10">
+        <v>1245</v>
+      </c>
+      <c r="R35" s="10">
+        <f>P35+Q35</f>
+        <v>24628</v>
+      </c>
+      <c r="S35" s="13">
+        <f>P35/R35</f>
+        <v>0.9494477830112068</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B36"/>
       <c r="C36"/>
       <c r="G36"/>
       <c r="I36"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <f>9300*30000</f>
         <v>279000000</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <f>14000*14693</f>
         <v>205702000</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <f>B39-B40</f>
         <v>73298000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N27:O27"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="B25:G25"/>
@@ -1943,7 +2335,7 @@
     <mergeCell ref="B17:G17"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G16 G26 G28:G1048576 G23:G24 G18:G21">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="percent" val="80"/>
         <cfvo type="percent" val="90"/>
@@ -1955,7 +2347,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32:M1048576 M1:M30">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S2">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S28 S30:S1048576">
     <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S29">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="90"/>
         <cfvo type="percent" val="95"/>

</xml_diff>

<commit_message>
Compare all failled files to darfeuille && create constants
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t xml:space="preserve">LIGNE </t>
   </si>
@@ -136,9 +136,6 @@
     <t>Il y a 414217 fichiers</t>
   </si>
   <si>
-    <t xml:space="preserve">Fichiers non traités : </t>
-  </si>
-  <si>
     <t>T1 T2 T3 T4 T5 T6 COMMUNS</t>
   </si>
   <si>
@@ -160,7 +157,7 @@
     <t>Analyse Dernière semaine</t>
   </si>
   <si>
-    <t>Il faut 4 jours pour faire la comparaison classique station sur station et ligne par ligne</t>
+    <t>Il faut 4/5 jours pour faire la comparaison classique station sur station et ligne par ligne</t>
   </si>
 </sst>
 </file>
@@ -305,7 +302,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -329,6 +326,13 @@
     <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -344,16 +348,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
@@ -665,9 +665,9 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,6 +681,7 @@
     <col min="9" max="9" width="31.7109375" style="7" customWidth="1"/>
     <col min="10" max="12" width="14.28515625" style="17" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" style="5" customWidth="1"/>
+    <col min="14" max="15" width="16.140625" customWidth="1"/>
     <col min="19" max="19" width="23.42578125" style="5"/>
   </cols>
   <sheetData>
@@ -694,30 +695,32 @@
       <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="I1" s="24"/>
       <c r="M1" s="5">
         <v>1</v>
       </c>
-      <c r="N1" t="s">
-        <v>47</v>
-      </c>
+      <c r="N1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="25"/>
       <c r="S1" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="27"/>
       <c r="G2" s="5">
         <v>0.01</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
       <c r="M2" s="5">
         <v>0.01</v>
       </c>
@@ -1537,16 +1540,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
       <c r="H17">
         <v>100666</v>
       </c>
@@ -1802,14 +1805,14 @@
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
+      <c r="B22" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
       <c r="H22">
         <v>106666</v>
       </c>
@@ -1848,7 +1851,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="15"/>
@@ -1965,27 +1968,21 @@
       <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
       <c r="H25" s="17"/>
-      <c r="I25" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="17">
-        <f>414217-L24</f>
-        <v>295</v>
-      </c>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
       <c r="M25" s="5">
         <f>1-L25/414217</f>
-        <v>0.99928781290965851</v>
+        <v>1</v>
       </c>
       <c r="Q25">
         <f>(Q24*5)/3600</f>
@@ -1999,17 +1996,17 @@
       <c r="F26" s="3"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
       <c r="H27" s="17">
         <f>K24*5</f>
         <v>337000</v>
@@ -2019,18 +2016,18 @@
         <v>6.9681134259259263</v>
       </c>
       <c r="K27" s="7"/>
-      <c r="N27" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23" t="str">
+      <c r="N27" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26" t="str">
         <f>CONCATENATE("Il faut ",Q25," heures de plus pour faire la comparaison des erreurs sur darfeuille")</f>
         <v>Il faut 107,697222222222 heures de plus pour faire la comparaison des erreurs sur darfeuille</v>
       </c>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="31" t="str">
-        <f>CONCATENATE("Soit ",((Q25/24)+4)," jours")</f>
-        <v>Soit 8,48738425925926 jours</v>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="23" t="str">
+        <f>CONCATENATE("Soit minimum ",((Q25/24)+4)," jours")</f>
+        <v>Soit minimum 8,48738425925926 jours</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2323,7 +2320,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="P27:Q27"/>
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="B2:C2"/>
@@ -2412,21 +2410,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004955207F9F5B314B8B9B51B8E365D485" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c516aae3580213d3db2e32983502eaaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c1ef9b3-4174-4af3-a5b1-5f98b740a774" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c89a2e4264c97434fad65ccc84a3a390" ns2:_="">
     <xsd:import namespace="4c1ef9b3-4174-4af3-a5b1-5f98b740a774"/>
@@ -2574,24 +2557,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE5D3DB7-DCDC-44A8-A58C-499D0DB8587A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2607,4 +2588,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
append constants && clean code && rename few output
</commit_message>
<xml_diff>
--- a/STATS.xlsx
+++ b/STATS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t xml:space="preserve">LIGNE </t>
   </si>
@@ -158,18 +158,40 @@
   </si>
   <si>
     <t>Il faut 4/5 jours pour faire la comparaison classique station sur station et ligne par ligne</t>
+  </si>
+  <si>
+    <t>Analyse T1 à T6 + Liaison B/D</t>
+  </si>
+  <si>
+    <t>ANALYSE 1</t>
+  </si>
+  <si>
+    <t>ANALYSE 2</t>
+  </si>
+  <si>
+    <t>ANALYSE 3</t>
+  </si>
+  <si>
+    <t>ANALYSE 4</t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>16h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="hh:\ mm:\ ss"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="166" formatCode="dd:\ hh:\ mm:\ ss"/>
+    <numFmt numFmtId="168" formatCode="dd:hh:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,8 +228,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +262,32 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -295,14 +350,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -330,6 +391,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -354,12 +428,23 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="9"/>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="40 % - Accent5" xfId="9" builtinId="47"/>
+    <cellStyle name="Accent1" xfId="7" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="8" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="6" builtinId="37"/>
     <cellStyle name="Accent4" xfId="2" builtinId="41"/>
+    <cellStyle name="Accent6" xfId="10" builtinId="49"/>
     <cellStyle name="Neutre" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Titre" xfId="5" builtinId="15"/>
     <cellStyle name="Vérification" xfId="1" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,11 +748,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I24" sqref="I24"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,453 +770,483 @@
     <col min="19" max="19" width="23.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:26" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="B1" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="H1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="N1" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="T1" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+    </row>
+    <row r="2" spans="1:26" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="M1" s="5">
+      <c r="I2" s="24"/>
+      <c r="M2" s="5">
         <v>1</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="S1" s="5">
+      <c r="O2" s="30"/>
+      <c r="S2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="Z2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="G2" s="5">
+      <c r="C3" s="32"/>
+      <c r="G3" s="5">
         <v>0.01</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H3" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="M2" s="5">
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="M3" s="5">
         <v>0.01</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S3" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="Z3" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="18" t="s">
+      <c r="P4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="T4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="3">
         <v>8289</v>
       </c>
-      <c r="C4" s="7">
-        <f t="shared" ref="C4:C35" si="0">B4/86400</f>
+      <c r="C5" s="7">
+        <f t="shared" ref="C5:C36" si="0">B5/86400</f>
         <v>9.5937499999999995E-2</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>73284</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>3681</v>
       </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F19" si="1">D4+E4</f>
+      <c r="F5">
+        <f t="shared" ref="F5:F20" si="1">D5+E5</f>
         <v>76965</v>
       </c>
-      <c r="G4" s="5">
-        <f>D4/F4</f>
+      <c r="G5" s="5">
+        <f>D5/F5</f>
         <v>0.95217306567920479</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <v>1817</v>
       </c>
-      <c r="I4" s="22">
-        <f t="shared" ref="I4:I34" si="2">H4/86400</f>
+      <c r="I5" s="22">
+        <f t="shared" ref="I5:I35" si="2">H5/86400</f>
         <v>2.1030092592592593E-2</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J5" s="17">
         <v>66802</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K5" s="17">
         <v>58</v>
       </c>
-      <c r="L4" s="17">
-        <f t="shared" ref="L4:L13" si="3">J4+K4</f>
+      <c r="L5" s="17">
+        <f t="shared" ref="L5:L14" si="3">J5+K5</f>
         <v>66860</v>
       </c>
-      <c r="M4" s="5">
-        <f>J4/L4</f>
+      <c r="M5" s="5">
+        <f>J5/L5</f>
         <v>0.99913251570445705</v>
       </c>
-      <c r="P4">
+      <c r="P5">
         <v>66528</v>
       </c>
-      <c r="Q4">
+      <c r="Q5">
         <v>2592</v>
       </c>
-      <c r="R4" s="17">
-        <f>P4+Q4</f>
+      <c r="R5" s="17">
+        <f>P5+Q5</f>
         <v>69120</v>
       </c>
-      <c r="S4" s="5">
-        <f>P4/R4</f>
+      <c r="S5" s="5">
+        <f>P5/R5</f>
         <v>0.96250000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="3">
         <v>1794</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C6" s="7">
         <f t="shared" si="0"/>
         <v>2.0763888888888887E-2</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>29810</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>4649</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <f t="shared" si="1"/>
         <v>34459</v>
       </c>
-      <c r="G5" s="5">
-        <f t="shared" ref="G5:G19" si="4">D5/F5</f>
+      <c r="G6" s="5">
+        <f t="shared" ref="G6:G20" si="4">D6/F6</f>
         <v>0.86508604428451208</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>13000</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I6" s="22">
         <f t="shared" si="2"/>
         <v>0.15046296296296297</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J6" s="17">
         <v>33166</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K6" s="20">
         <v>1293</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L6" s="17">
         <f t="shared" si="3"/>
         <v>34459</v>
       </c>
-      <c r="M5" s="5">
-        <f t="shared" ref="M5:M8" si="5">J5/L5</f>
+      <c r="M6" s="5">
+        <f t="shared" ref="M6:M9" si="5">J6/L6</f>
         <v>0.96247714675411356</v>
       </c>
-      <c r="P5">
+      <c r="P6">
         <v>29913</v>
       </c>
-      <c r="Q5">
+      <c r="Q6">
         <v>2015</v>
       </c>
-      <c r="R5" s="17">
-        <f t="shared" ref="R5:R23" si="6">P5+Q5</f>
+      <c r="R6" s="17">
+        <f t="shared" ref="R6:R24" si="6">P6+Q6</f>
         <v>31928</v>
       </c>
-      <c r="S5" s="5">
-        <f t="shared" ref="S5:S23" si="7">P5/R5</f>
+      <c r="S6" s="5">
+        <f t="shared" ref="S6:S24" si="7">P6/R6</f>
         <v>0.93688925081433228</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="3">
         <v>940</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C7" s="7">
         <f t="shared" si="0"/>
         <v>1.087962962962963E-2</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>8757</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>179</v>
       </c>
-      <c r="F6">
-        <f>D6+E6</f>
+      <c r="F7">
+        <f>D7+E7</f>
         <v>8936</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G7" s="5">
         <f t="shared" si="4"/>
         <v>0.97996866606982991</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>1500</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I7" s="22">
         <f t="shared" si="2"/>
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J7" s="17">
         <v>7198</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K7" s="17">
         <v>174</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L7" s="17">
         <f t="shared" si="3"/>
         <v>7372</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M7" s="5">
         <f t="shared" si="5"/>
         <v>0.97639717851329355</v>
       </c>
-      <c r="P6">
+      <c r="P7">
         <v>6997</v>
       </c>
-      <c r="Q6">
+      <c r="Q7">
         <v>297</v>
       </c>
-      <c r="R6" s="17">
+      <c r="R7" s="17">
         <f t="shared" si="6"/>
         <v>7294</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S7" s="5">
         <f t="shared" si="7"/>
         <v>0.95928160131615026</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>4000</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="7">
         <f t="shared" si="0"/>
         <v>4.6296296296296294E-2</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>32400</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>2532</v>
       </c>
-      <c r="F7">
-        <f>D7+E7</f>
+      <c r="F8">
+        <f>D8+E8</f>
         <v>34932</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G8" s="5">
         <f t="shared" si="4"/>
         <v>0.92751631741669527</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>4400</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I8" s="22">
         <f t="shared" si="2"/>
         <v>5.0925925925925923E-2</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J8" s="17">
         <v>30377</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K8" s="20">
         <v>2137</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L8" s="17">
         <f t="shared" si="3"/>
         <v>32514</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M8" s="5">
         <f t="shared" si="5"/>
         <v>0.93427446638371159</v>
       </c>
-      <c r="P7">
+      <c r="P8">
         <v>27056</v>
       </c>
-      <c r="Q7">
+      <c r="Q8">
         <v>2606</v>
       </c>
-      <c r="R7" s="17">
+      <c r="R8" s="17">
         <f t="shared" si="6"/>
         <v>29662</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S8" s="5">
         <f t="shared" si="7"/>
         <v>0.9121434832445553</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="3">
         <v>923</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C9" s="7">
         <f t="shared" si="0"/>
         <v>1.068287037037037E-2</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>20430</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>25490</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <f t="shared" si="1"/>
         <v>45920</v>
       </c>
-      <c r="G8" s="5">
-        <f>D8/F8</f>
+      <c r="G9" s="5">
+        <f>D9/F9</f>
         <v>0.44490418118466901</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>25298</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I9" s="22">
         <f t="shared" si="2"/>
         <v>0.29280092592592594</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J9" s="17">
         <v>24640</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K9" s="20">
         <v>21292</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L9" s="17">
         <f t="shared" si="3"/>
         <v>45932</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M9" s="5">
         <f t="shared" si="5"/>
         <v>0.53644517983105455</v>
       </c>
-      <c r="P8">
+      <c r="P9">
         <v>20390</v>
       </c>
-      <c r="Q8">
+      <c r="Q9">
         <v>25514</v>
       </c>
-      <c r="R8" s="17">
+      <c r="R9" s="17">
         <f t="shared" si="6"/>
         <v>45904</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S9" s="5">
         <f t="shared" si="7"/>
         <v>0.44418787033809692</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="16"/>
-      <c r="H9">
-        <v>180</v>
-      </c>
-      <c r="I9" s="22">
-        <f t="shared" si="2"/>
-        <v>2.0833333333333333E-3</v>
-      </c>
-      <c r="J9" s="17">
-        <v>7261</v>
-      </c>
-      <c r="K9" s="17">
-        <v>159</v>
-      </c>
-      <c r="L9" s="17">
-        <f t="shared" si="3"/>
-        <v>7420</v>
-      </c>
-      <c r="M9" s="5">
-        <f>J9/L9</f>
-        <v>0.97857142857142854</v>
-      </c>
-      <c r="R9" s="17"/>
-      <c r="S9" s="5" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="15"/>
@@ -1140,624 +1255,681 @@
       <c r="F10" s="9"/>
       <c r="G10" s="16"/>
       <c r="H10">
-        <v>2856</v>
+        <v>180</v>
       </c>
       <c r="I10" s="22">
         <f t="shared" si="2"/>
-        <v>3.3055555555555553E-2</v>
+        <v>2.0833333333333333E-3</v>
       </c>
       <c r="J10" s="17">
-        <v>39723</v>
-      </c>
-      <c r="K10" s="20">
-        <v>4626</v>
+        <v>7261</v>
+      </c>
+      <c r="K10" s="17">
+        <v>159</v>
       </c>
       <c r="L10" s="17">
         <f t="shared" si="3"/>
+        <v>7420</v>
+      </c>
+      <c r="M10" s="5">
+        <f>J10/L10</f>
+        <v>0.97857142857142854</v>
+      </c>
+      <c r="R10" s="17"/>
+      <c r="S10" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="16"/>
+      <c r="H11">
+        <v>2856</v>
+      </c>
+      <c r="I11" s="22">
+        <f t="shared" si="2"/>
+        <v>3.3055555555555553E-2</v>
+      </c>
+      <c r="J11" s="17">
+        <v>39723</v>
+      </c>
+      <c r="K11" s="20">
+        <v>4626</v>
+      </c>
+      <c r="L11" s="17">
+        <f t="shared" si="3"/>
         <v>44349</v>
       </c>
-      <c r="M10" s="5">
-        <f t="shared" ref="M10:M11" si="8">J10/L10</f>
+      <c r="M11" s="5">
+        <f t="shared" ref="M11:M12" si="8">J11/L11</f>
         <v>0.89569099641480077</v>
       </c>
-      <c r="P10">
+      <c r="P11">
         <v>39312</v>
       </c>
-      <c r="Q10">
+      <c r="Q11">
         <v>4110</v>
       </c>
-      <c r="R10" s="17">
+      <c r="R11" s="17">
         <f t="shared" si="6"/>
         <v>43422</v>
       </c>
-      <c r="S10" s="5">
+      <c r="S11" s="5">
         <f t="shared" si="7"/>
         <v>0.90534751969047944</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>500</v>
       </c>
-      <c r="C11" s="7">
-        <f>B11/86400</f>
+      <c r="C12" s="7">
+        <f>B12/86400</f>
         <v>5.7870370370370367E-3</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>4612</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>361</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <f t="shared" si="1"/>
         <v>4973</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G12" s="5">
         <f t="shared" si="4"/>
         <v>0.92740800321737382</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>260</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I12" s="22">
         <f t="shared" si="2"/>
         <v>3.0092592592592593E-3</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J12" s="17">
         <v>4675</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K12" s="17">
         <v>301</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L12" s="17">
         <f t="shared" si="3"/>
         <v>4976</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M12" s="5">
         <f t="shared" si="8"/>
         <v>0.93950964630225076</v>
       </c>
-      <c r="P11">
+      <c r="P12">
         <v>4610</v>
       </c>
-      <c r="Q11">
+      <c r="Q12">
         <v>56</v>
       </c>
-      <c r="R11" s="17">
+      <c r="R12" s="17">
         <f t="shared" si="6"/>
         <v>4666</v>
       </c>
-      <c r="S11" s="5">
+      <c r="S12" s="5">
         <f t="shared" si="7"/>
         <v>0.98799828546935275</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="T12" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="U12" s="26"/>
+      <c r="V12" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="W12" s="29">
+        <v>30682</v>
+      </c>
+      <c r="X12" s="29">
+        <v>373</v>
+      </c>
+      <c r="Y12" s="29">
+        <f>W12+X12</f>
+        <v>31055</v>
+      </c>
+      <c r="Z12" s="27">
+        <f>W12/Y12</f>
+        <v>0.98798905168249884</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>750</v>
       </c>
-      <c r="C12" s="7">
-        <f>B12/86400</f>
+      <c r="C13" s="7">
+        <f>B13/86400</f>
         <v>8.6805555555555559E-3</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>7810</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>242</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <f t="shared" si="1"/>
         <v>8052</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G13" s="5">
         <f t="shared" si="4"/>
         <v>0.9699453551912568</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>914</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I13" s="22">
         <f t="shared" si="2"/>
         <v>1.0578703703703703E-2</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J13" s="17">
         <v>7223</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K13" s="17">
         <v>140</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L13" s="17">
         <f t="shared" si="3"/>
         <v>7363</v>
       </c>
-      <c r="M12" s="5">
-        <f t="shared" ref="M12" si="9">J12/L12</f>
+      <c r="M13" s="5">
+        <f t="shared" ref="M13" si="9">J13/L13</f>
         <v>0.98098601113676487</v>
       </c>
-      <c r="P12">
+      <c r="P13">
         <v>7123</v>
       </c>
-      <c r="Q12">
+      <c r="Q13">
         <v>95</v>
       </c>
-      <c r="R12" s="17">
+      <c r="R13" s="17">
         <f t="shared" si="6"/>
         <v>7218</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S13" s="5">
         <f t="shared" si="7"/>
         <v>0.98683845940703796</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="T13" s="29"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="27"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <v>1216</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>1.4074074074074074E-2</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>11000</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>802</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <f t="shared" si="1"/>
         <v>11802</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G14" s="5">
         <f t="shared" si="4"/>
         <v>0.93204541603118118</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>483</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I14" s="22">
         <f t="shared" si="2"/>
         <v>5.5902777777777773E-3</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J14" s="17">
         <v>10134</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K14" s="17">
         <v>674</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L14" s="17">
         <f t="shared" si="3"/>
         <v>10808</v>
       </c>
-      <c r="M13" s="5">
-        <f t="shared" ref="M13:M14" si="10">J13/L13</f>
+      <c r="M14" s="5">
+        <f t="shared" ref="M14:M15" si="10">J14/L14</f>
         <v>0.93763878608438189</v>
       </c>
-      <c r="P13">
+      <c r="P14">
         <v>10070</v>
       </c>
-      <c r="Q13">
+      <c r="Q14">
         <v>385</v>
       </c>
-      <c r="R13" s="17">
+      <c r="R14" s="17">
         <f t="shared" si="6"/>
         <v>10455</v>
       </c>
-      <c r="S13" s="5">
+      <c r="S14" s="5">
         <f t="shared" si="7"/>
         <v>0.96317551410808222</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="T14" s="29"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="29"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="27"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B15" s="3">
         <v>224</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
         <v>2.5925925925925925E-3</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>5980</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>822</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <f t="shared" si="1"/>
         <v>6802</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G15" s="5">
         <f t="shared" si="4"/>
         <v>0.87915319023816529</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>1451</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I15" s="22">
         <f t="shared" si="2"/>
         <v>1.6793981481481483E-2</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J15" s="17">
         <v>6762</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K15" s="17">
         <v>42</v>
       </c>
-      <c r="L14" s="17">
-        <f>J14+K14</f>
+      <c r="L15" s="17">
+        <f>J15+K15</f>
         <v>6804</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M15" s="5">
         <f t="shared" si="10"/>
         <v>0.99382716049382713</v>
       </c>
-      <c r="P14">
+      <c r="P15">
         <v>6395</v>
       </c>
-      <c r="Q14">
+      <c r="Q15">
         <v>22</v>
       </c>
-      <c r="R14" s="17">
+      <c r="R15" s="17">
         <f t="shared" si="6"/>
         <v>6417</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S15" s="5">
         <f t="shared" si="7"/>
         <v>0.99657160666978339</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="T15" s="29"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="27"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>131</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
         <v>1.5162037037037036E-3</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>749</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>42</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G16" s="5">
         <f t="shared" si="4"/>
         <v>0.94690265486725667</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>149</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I16" s="22">
         <f t="shared" si="2"/>
         <v>1.724537037037037E-3</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J16" s="17">
         <v>776</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K16" s="17">
         <v>3</v>
       </c>
-      <c r="L15" s="17">
-        <f t="shared" ref="L15:L23" si="11">J15+K15</f>
+      <c r="L16" s="17">
+        <f t="shared" ref="L16:L24" si="11">J16+K16</f>
         <v>779</v>
       </c>
-      <c r="M15" s="5">
-        <f>J15/L15</f>
+      <c r="M16" s="5">
+        <f>J16/L16</f>
         <v>0.99614890885750962</v>
       </c>
-      <c r="P15">
+      <c r="P16">
         <v>779</v>
       </c>
-      <c r="Q15">
+      <c r="Q16">
         <v>3</v>
       </c>
-      <c r="R15" s="17">
+      <c r="R16" s="17">
         <f t="shared" si="6"/>
         <v>782</v>
       </c>
-      <c r="S15" s="5">
+      <c r="S16" s="5">
         <f t="shared" si="7"/>
         <v>0.99616368286445012</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="T16" s="29"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="27"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B17" s="3">
         <v>99</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C17" s="7">
         <f t="shared" si="0"/>
         <v>1.1458333333333333E-3</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>1193</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>24</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <f t="shared" si="1"/>
         <v>1217</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G17" s="5">
         <f t="shared" si="4"/>
         <v>0.98027937551355793</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I17" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J17" s="17">
         <v>1143</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K17" s="17">
         <v>23</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L17" s="17">
         <f t="shared" si="11"/>
         <v>1166</v>
       </c>
-      <c r="M16" s="5">
-        <f t="shared" ref="M16:M23" si="12">J16/L16</f>
+      <c r="M17" s="5">
+        <f t="shared" ref="M17:M24" si="12">J17/L17</f>
         <v>0.98027444253859353</v>
       </c>
-      <c r="P16">
+      <c r="P17">
         <v>1142</v>
       </c>
-      <c r="Q16">
+      <c r="Q17">
         <v>21</v>
       </c>
-      <c r="R16" s="17">
+      <c r="R17" s="17">
         <f t="shared" si="6"/>
         <v>1163</v>
       </c>
-      <c r="S16" s="5">
+      <c r="S17" s="5">
         <f t="shared" si="7"/>
         <v>0.98194325021496132</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="T17" s="29"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="27"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B18" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17">
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18">
         <v>100666</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I18" s="22">
         <f t="shared" si="2"/>
         <v>1.1651157407407406</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J18" s="17">
         <f>42780+3456</f>
         <v>46236</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K18" s="20">
         <v>11388</v>
       </c>
-      <c r="L17" s="17">
+      <c r="L18" s="17">
         <f t="shared" si="11"/>
         <v>57624</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M18" s="5">
         <f t="shared" si="12"/>
         <v>0.80237401082882132</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>43356</v>
       </c>
-      <c r="Q17">
+      <c r="Q18">
         <v>13482</v>
       </c>
-      <c r="R17" s="17">
+      <c r="R18" s="17">
         <f t="shared" si="6"/>
         <v>56838</v>
       </c>
-      <c r="S17" s="5">
+      <c r="S18" s="5">
         <f t="shared" si="7"/>
         <v>0.76279953552200996</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="T18" s="39"/>
+      <c r="U18" s="39"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B19" s="3">
         <v>577</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C19" s="7">
         <f t="shared" si="0"/>
         <v>6.6782407407407407E-3</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>7638</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>2398</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <f t="shared" si="1"/>
         <v>10036</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G19" s="5">
         <f t="shared" si="4"/>
         <v>0.76106018333997605</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>1994</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I19" s="22">
         <f t="shared" si="2"/>
         <v>2.3078703703703702E-2</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J19" s="17">
         <v>6565</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K19" s="20">
         <v>30</v>
       </c>
-      <c r="L18" s="17">
+      <c r="L19" s="17">
         <f t="shared" si="11"/>
         <v>6595</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M19" s="5">
         <f t="shared" si="12"/>
         <v>0.99545109931766484</v>
       </c>
-      <c r="P18">
+      <c r="P19">
         <v>6763</v>
       </c>
-      <c r="Q18">
+      <c r="Q19">
         <v>1616</v>
       </c>
-      <c r="R18" s="17">
+      <c r="R19" s="17">
         <f t="shared" si="6"/>
         <v>8379</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S19" s="5">
         <f t="shared" si="7"/>
         <v>0.80713688984365672</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="3">
         <v>21</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C20" s="7">
         <f t="shared" si="0"/>
         <v>2.4305555555555555E-4</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>388</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>378</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <f t="shared" si="1"/>
         <v>766</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G20" s="5">
         <f t="shared" si="4"/>
         <v>0.50652741514360311</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <v>2821</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I20" s="22">
         <f t="shared" si="2"/>
         <v>3.2650462962962964E-2</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J20" s="17">
         <v>516</v>
       </c>
-      <c r="K19" s="17">
+      <c r="K20" s="17">
         <v>248</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L20" s="17">
         <f t="shared" si="11"/>
         <v>764</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M20" s="5">
         <f t="shared" si="12"/>
         <v>0.67539267015706805</v>
       </c>
-      <c r="P19">
+      <c r="P20">
         <v>303</v>
       </c>
-      <c r="Q19">
+      <c r="Q20">
         <v>377</v>
       </c>
-      <c r="R19" s="17">
+      <c r="R20" s="17">
         <f t="shared" si="6"/>
         <v>680</v>
       </c>
-      <c r="S19" s="5">
+      <c r="S20" s="5">
         <f t="shared" si="7"/>
         <v>0.44558823529411767</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>33</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="16"/>
-      <c r="H20">
-        <v>300</v>
-      </c>
-      <c r="I20" s="22">
-        <f t="shared" si="2"/>
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="J20" s="17">
-        <v>3054</v>
-      </c>
-      <c r="K20" s="17">
-        <v>115</v>
-      </c>
-      <c r="L20" s="17">
-        <f t="shared" si="11"/>
-        <v>3169</v>
-      </c>
-      <c r="M20" s="5">
-        <f t="shared" si="12"/>
-        <v>0.96371094982644367</v>
-      </c>
-      <c r="P20">
-        <v>3027</v>
-      </c>
-      <c r="Q20">
-        <v>102</v>
-      </c>
-      <c r="R20" s="17">
-        <f t="shared" si="6"/>
-        <v>3129</v>
-      </c>
-      <c r="S20" s="5">
-        <f t="shared" si="7"/>
-        <v>0.96740172579098749</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>36</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="15"/>
@@ -1766,574 +1938,679 @@
       <c r="F21" s="9"/>
       <c r="G21" s="16"/>
       <c r="H21">
-        <v>176</v>
+        <v>300</v>
       </c>
       <c r="I21" s="22">
         <f t="shared" si="2"/>
-        <v>2.0370370370370369E-3</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="J21" s="17">
-        <v>11661</v>
+        <v>3054</v>
       </c>
       <c r="K21" s="17">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="L21" s="17">
         <f t="shared" si="11"/>
-        <v>11683</v>
+        <v>3169</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="12"/>
-        <v>0.99811692202345292</v>
+        <v>0.96371094982644367</v>
       </c>
       <c r="P21">
-        <v>11661</v>
+        <v>3027</v>
       </c>
       <c r="Q21">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="R21" s="17">
         <f t="shared" si="6"/>
-        <v>11683</v>
+        <v>3129</v>
       </c>
       <c r="S21" s="5">
         <f t="shared" si="7"/>
-        <v>0.99811692202345292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0.96740172579098749</v>
+      </c>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
+        <v>36</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="16"/>
       <c r="H22">
-        <v>106666</v>
+        <v>176</v>
       </c>
       <c r="I22" s="22">
         <f t="shared" si="2"/>
-        <v>1.2345601851851853</v>
+        <v>2.0370370370370369E-3</v>
       </c>
       <c r="J22" s="17">
-        <v>38256</v>
-      </c>
-      <c r="K22" s="20">
-        <v>24660</v>
+        <v>11661</v>
+      </c>
+      <c r="K22" s="17">
+        <v>22</v>
       </c>
       <c r="L22" s="17">
         <f t="shared" si="11"/>
-        <v>62916</v>
+        <v>11683</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="12"/>
-        <v>0.60804882700743845</v>
+        <v>0.99811692202345292</v>
       </c>
       <c r="P22">
-        <v>38110</v>
+        <v>11661</v>
       </c>
       <c r="Q22">
-        <v>24195</v>
+        <v>22</v>
       </c>
       <c r="R22" s="17">
         <f t="shared" si="6"/>
-        <v>62305</v>
+        <v>11683</v>
       </c>
       <c r="S22" s="5">
         <f t="shared" si="7"/>
-        <v>0.61166840542492573</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0.99811692202345292</v>
+      </c>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="16"/>
+        <v>37</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
       <c r="H23">
-        <v>114</v>
+        <v>106666</v>
       </c>
       <c r="I23" s="22">
         <f t="shared" si="2"/>
-        <v>1.3194444444444445E-3</v>
+        <v>1.2345601851851853</v>
       </c>
       <c r="J23" s="17">
-        <v>354</v>
-      </c>
-      <c r="K23" s="17">
-        <v>15</v>
+        <v>38256</v>
+      </c>
+      <c r="K23" s="20">
+        <v>24660</v>
       </c>
       <c r="L23" s="17">
         <f t="shared" si="11"/>
-        <v>369</v>
+        <v>62916</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="12"/>
-        <v>0.95934959349593496</v>
+        <v>0.60804882700743845</v>
       </c>
       <c r="P23">
-        <v>338</v>
+        <v>38110</v>
       </c>
       <c r="Q23">
-        <v>32</v>
+        <v>24195</v>
       </c>
       <c r="R23" s="17">
         <f t="shared" si="6"/>
-        <v>370</v>
+        <v>62305</v>
       </c>
       <c r="S23" s="5">
         <f t="shared" si="7"/>
+        <v>0.61166840542492573</v>
+      </c>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="16"/>
+      <c r="H24">
+        <v>114</v>
+      </c>
+      <c r="I24" s="22">
+        <f t="shared" si="2"/>
+        <v>1.3194444444444445E-3</v>
+      </c>
+      <c r="J24" s="17">
+        <v>354</v>
+      </c>
+      <c r="K24" s="17">
+        <v>15</v>
+      </c>
+      <c r="L24" s="17">
+        <f t="shared" si="11"/>
+        <v>369</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" si="12"/>
+        <v>0.95934959349593496</v>
+      </c>
+      <c r="P24">
+        <v>338</v>
+      </c>
+      <c r="Q24">
+        <v>32</v>
+      </c>
+      <c r="R24" s="17">
+        <f t="shared" si="6"/>
+        <v>370</v>
+      </c>
+      <c r="S24" s="5">
+        <f t="shared" si="7"/>
         <v>0.91351351351351351</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="25"/>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="25"/>
+    </row>
+    <row r="25" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="11">
-        <f>SUM(B4:B19)</f>
+      <c r="B25" s="11">
+        <f>SUM(B5:B20)</f>
         <v>19464</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C25" s="12">
         <f t="shared" si="0"/>
         <v>0.22527777777777777</v>
       </c>
-      <c r="D24" s="11">
-        <f>SUM(D4:D19)</f>
+      <c r="D25" s="11">
+        <f>SUM(D5:D20)</f>
         <v>204051</v>
       </c>
-      <c r="E24" s="11">
-        <f>SUM(E4:E19)</f>
+      <c r="E25" s="11">
+        <f>SUM(E5:E20)</f>
         <v>41600</v>
       </c>
-      <c r="F24" s="11">
-        <f>SUM(F4:F19)</f>
+      <c r="F25" s="11">
+        <f>SUM(F5:F20)</f>
         <v>245651</v>
       </c>
-      <c r="G24" s="13">
-        <f>D24/F24</f>
+      <c r="G25" s="13">
+        <f>D25/F25</f>
         <v>0.83065405799284353</v>
       </c>
-      <c r="H24" s="11">
-        <f>SUM(H4:H23)</f>
+      <c r="H25" s="11">
+        <f>SUM(H5:H24)</f>
         <v>265045</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I25" s="21">
         <f t="shared" si="2"/>
         <v>3.0676504629629631</v>
       </c>
-      <c r="J24" s="19">
-        <f>SUM(J4:J23)</f>
+      <c r="J25" s="19">
+        <f>SUM(J5:J24)</f>
         <v>346522</v>
       </c>
-      <c r="K24" s="19">
-        <f>SUM(K4:K23)</f>
+      <c r="K25" s="19">
+        <f>SUM(K5:K24)</f>
         <v>67400</v>
       </c>
-      <c r="L24" s="19">
-        <f>SUM(L4:L23)</f>
+      <c r="L25" s="19">
+        <f>SUM(L5:L24)</f>
         <v>413922</v>
       </c>
-      <c r="M24" s="13">
-        <f>J24/L24</f>
+      <c r="M25" s="13">
+        <f>J25/L25</f>
         <v>0.83716738902498533</v>
       </c>
-      <c r="P24" s="19">
-        <f>SUM(P4:P23)</f>
+      <c r="P25" s="19">
+        <f>SUM(P5:P24)</f>
         <v>323873</v>
       </c>
-      <c r="Q24" s="19">
-        <f>SUM(Q4:Q23)</f>
+      <c r="Q25" s="19">
+        <f>SUM(Q5:Q24)</f>
         <v>77542</v>
       </c>
-      <c r="R24" s="19">
-        <f>SUM(R4:R23)</f>
+      <c r="R25" s="19">
+        <f>SUM(R5:R24)</f>
         <v>401415</v>
       </c>
-      <c r="S24" s="13">
-        <f>P24/R24</f>
+      <c r="S25" s="13">
+        <f>P25/R25</f>
         <v>0.80682834473051579</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="W25" s="10">
+        <f>SUM(W5:W23)</f>
+        <v>30682</v>
+      </c>
+      <c r="X25" s="10">
+        <f t="shared" ref="X25:Y25" si="13">SUM(X5:X23)</f>
+        <v>373</v>
+      </c>
+      <c r="Y25" s="10">
+        <f t="shared" si="13"/>
+        <v>31055</v>
+      </c>
+      <c r="Z25" s="10">
+        <f>W25/Y25</f>
+        <v>0.98798905168249884</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B26" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="M25" s="5">
-        <f>1-L25/414217</f>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="M26" s="5">
+        <f>1-L26/414217</f>
         <v>1</v>
       </c>
-      <c r="Q25">
-        <f>(Q24*5)/3600</f>
+      <c r="Q26">
+        <f>(Q25*5)/3600</f>
         <v>107.69722222222222</v>
       </c>
-      <c r="R25" s="17">
+      <c r="R26" s="17">
         <v>414217</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
-      <c r="I26"/>
-    </row>
-    <row r="27" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C28" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="17">
-        <f>K24*5</f>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="17">
+        <f>K25*5</f>
         <v>337000</v>
       </c>
-      <c r="I27" s="22">
-        <f>(H27/86400)+I24</f>
+      <c r="I28" s="22">
+        <f>(H28/86400)+I25</f>
         <v>6.9681134259259263</v>
       </c>
-      <c r="K27" s="7"/>
-      <c r="N27" s="26" t="s">
+      <c r="K28" s="7"/>
+      <c r="N28" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26" t="str">
-        <f>CONCATENATE("Il faut ",Q25," heures de plus pour faire la comparaison des erreurs sur darfeuille")</f>
+      <c r="O28" s="31"/>
+      <c r="P28" s="31" t="str">
+        <f>CONCATENATE("Il faut ",Q26," heures de plus pour faire la comparaison des erreurs sur darfeuille")</f>
         <v>Il faut 107,697222222222 heures de plus pour faire la comparaison des erreurs sur darfeuille</v>
       </c>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="23" t="str">
-        <f>CONCATENATE("Soit minimum ",((Q25/24)+4)," jours")</f>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="23" t="str">
+        <f>CONCATENATE("Soit minimum ",((Q26/24)+4)," jours")</f>
         <v>Soit minimum 8,48738425925926 jours</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F28" s="3"/>
-      <c r="I28"/>
-      <c r="S28"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+      <c r="I29"/>
+      <c r="S29"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B30" s="3">
         <v>877</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C30" s="7">
         <f t="shared" si="0"/>
         <v>1.0150462962962964E-2</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>19116</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>554</v>
       </c>
-      <c r="F29" s="3">
-        <f>D29+E29</f>
+      <c r="F30" s="3">
+        <f>D30+E30</f>
         <v>19670</v>
       </c>
-      <c r="G29" s="5">
-        <f t="shared" ref="G29:G34" si="13">D29/F29</f>
+      <c r="G30" s="5">
+        <f t="shared" ref="G30:G35" si="14">D30/F30</f>
         <v>0.9718352821555668</v>
       </c>
-      <c r="I29"/>
-      <c r="P29">
+      <c r="I30"/>
+      <c r="P30">
         <v>7232</v>
       </c>
-      <c r="Q29">
+      <c r="Q30">
         <v>378</v>
       </c>
-      <c r="R29">
-        <f>P29+Q29</f>
+      <c r="R30">
+        <f>P30+Q30</f>
         <v>7610</v>
       </c>
-      <c r="S29" s="13">
-        <f t="shared" ref="S29" si="14">P29/R29</f>
+      <c r="S30" s="13">
+        <f t="shared" ref="S30" si="15">P30/R30</f>
         <v>0.95032851511169514</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B31" s="3">
         <v>995</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C31" s="7">
         <f t="shared" si="0"/>
         <v>1.1516203703703704E-2</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>10311</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>3564</v>
-      </c>
-      <c r="F30" s="3">
-        <f>D30+E30</f>
-        <v>13875</v>
-      </c>
-      <c r="G30" s="5">
-        <f t="shared" si="13"/>
-        <v>0.74313513513513518</v>
-      </c>
-      <c r="I30"/>
-      <c r="S30"/>
-    </row>
-    <row r="31" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="11">
-        <v>25678</v>
-      </c>
-      <c r="C31" s="12">
-        <f t="shared" si="0"/>
-        <v>0.29719907407407409</v>
-      </c>
-      <c r="D31" s="10">
-        <v>86365</v>
-      </c>
-      <c r="E31" s="10">
-        <v>10791</v>
       </c>
       <c r="F31" s="3">
         <f>D31+E31</f>
+        <v>13875</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="14"/>
+        <v>0.74313513513513518</v>
+      </c>
+      <c r="I31"/>
+      <c r="S31"/>
+    </row>
+    <row r="32" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="11">
+        <v>25678</v>
+      </c>
+      <c r="C32" s="12">
+        <f>B32/86400</f>
+        <v>0.29719907407407409</v>
+      </c>
+      <c r="D32" s="10">
+        <v>86365</v>
+      </c>
+      <c r="E32" s="10">
+        <v>10791</v>
+      </c>
+      <c r="F32" s="3">
+        <f>D32+E32</f>
         <v>97156</v>
       </c>
-      <c r="G31" s="5">
-        <f t="shared" si="13"/>
+      <c r="G32" s="5">
+        <f t="shared" si="14"/>
         <v>0.88893120342541887</v>
       </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="P31" s="10">
+      <c r="I32" s="12"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="P32" s="10">
         <v>68040</v>
       </c>
-      <c r="Q31" s="10">
+      <c r="Q32" s="10">
         <v>10562</v>
       </c>
-      <c r="R31" s="10">
-        <f>P31+Q31</f>
+      <c r="R32" s="10">
+        <f>P32+Q32</f>
         <v>78602</v>
       </c>
-      <c r="S31" s="13">
-        <f>P31/R31</f>
+      <c r="S32" s="13">
+        <f>P32/R32</f>
         <v>0.86562682883387188</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F32" s="3"/>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B34" s="3">
         <v>41</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>420</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>39</v>
       </c>
-      <c r="F33" s="3">
-        <f t="shared" ref="F33" si="15">D33+E33</f>
+      <c r="F34" s="3">
+        <f t="shared" ref="F34" si="16">D34+E34</f>
         <v>459</v>
       </c>
-      <c r="G33" s="5">
-        <f t="shared" si="13"/>
+      <c r="G34" s="5">
+        <f t="shared" si="14"/>
         <v>0.91503267973856206</v>
       </c>
-      <c r="H33">
+      <c r="H34">
         <v>93</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I34" s="14">
         <f t="shared" si="2"/>
         <v>1.0763888888888889E-3</v>
       </c>
-      <c r="J33" s="17">
+      <c r="J34" s="17">
         <v>453</v>
       </c>
-      <c r="K33" s="17">
+      <c r="K34" s="17">
         <v>5</v>
       </c>
-      <c r="L33" s="17">
-        <f t="shared" ref="L33:L34" si="16">J33+K33</f>
+      <c r="L34" s="17">
+        <f t="shared" ref="L34:L35" si="17">J34+K34</f>
         <v>458</v>
       </c>
-      <c r="M33" s="5">
-        <f t="shared" ref="M33:M34" si="17">J33/L33</f>
+      <c r="M34" s="5">
+        <f t="shared" ref="M34:M35" si="18">J34/L34</f>
         <v>0.98908296943231444</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>3748</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <v>419</v>
       </c>
-      <c r="F34" s="3">
-        <f t="shared" ref="F34" si="18">D34+E34</f>
+      <c r="F35" s="3">
+        <f t="shared" ref="F35" si="19">D35+E35</f>
         <v>4167</v>
       </c>
-      <c r="G34" s="5">
-        <f t="shared" si="13"/>
+      <c r="G35" s="5">
+        <f t="shared" si="14"/>
         <v>0.89944804415646751</v>
       </c>
-      <c r="H34">
+      <c r="H35">
         <v>855</v>
       </c>
-      <c r="I34" s="14">
+      <c r="I35" s="14">
         <f t="shared" si="2"/>
         <v>9.8958333333333329E-3</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J35" s="17">
         <v>4329</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K35" s="17">
         <v>38</v>
       </c>
-      <c r="L34" s="17">
-        <f t="shared" si="16"/>
+      <c r="L35" s="17">
+        <f t="shared" si="17"/>
         <v>4367</v>
       </c>
-      <c r="M34" s="5">
-        <f t="shared" si="17"/>
+      <c r="M35" s="5">
+        <f t="shared" si="18"/>
         <v>0.99129837416991073</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+    <row r="36" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B36" s="11">
         <v>71386</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C36" s="12">
         <f t="shared" si="0"/>
         <v>0.82622685185185185</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D36" s="10">
         <v>23533</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E36" s="10">
         <v>1209</v>
       </c>
-      <c r="F35" s="10">
-        <f>D35+E35</f>
+      <c r="F36" s="10">
+        <f>D36+E36</f>
         <v>24742</v>
       </c>
-      <c r="G35" s="13">
-        <f>D35/F35</f>
+      <c r="G36" s="13">
+        <f>D36/F36</f>
         <v>0.9511357206369736</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="13"/>
-      <c r="P35" s="10">
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="13"/>
+      <c r="P36" s="10">
         <v>23383</v>
       </c>
-      <c r="Q35" s="10">
+      <c r="Q36" s="10">
         <v>1245</v>
       </c>
-      <c r="R35" s="10">
-        <f>P35+Q35</f>
+      <c r="R36" s="10">
+        <f>P36+Q36</f>
         <v>24628</v>
       </c>
-      <c r="S35" s="13">
-        <f>P35/R35</f>
+      <c r="S36" s="13">
+        <f>P36/R36</f>
         <v>0.9494477830112068</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="G36"/>
-      <c r="I36"/>
-      <c r="M36"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="U36" s="10">
+        <v>15493</v>
+      </c>
+      <c r="V36" s="42">
+        <f>U36/86400</f>
+        <v>0.17931712962962962</v>
+      </c>
+      <c r="W36" s="10">
+        <v>23383</v>
+      </c>
+      <c r="X36" s="10">
+        <v>1245</v>
+      </c>
+      <c r="Y36" s="10">
+        <f>W36+X36</f>
+        <v>24628</v>
+      </c>
+      <c r="Z36" s="13">
+        <f>W36/Y36</f>
+        <v>0.9494477830112068</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="G37"/>
+      <c r="I37"/>
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
         <f>9300*30000</f>
         <v>279000000</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B40" s="3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
         <f>14000*14693</f>
         <v>205702000</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="3">
-        <f>B39-B40</f>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <f>B40-B41</f>
         <v>73298000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B17:G17"/>
+  <mergeCells count="20">
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="Z12:Z17"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="T1:Z1"/>
+    <mergeCell ref="T12:T17"/>
+    <mergeCell ref="W12:W17"/>
+    <mergeCell ref="X12:X17"/>
+    <mergeCell ref="Y12:Y17"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="V12:V17"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:G16 G26 G28:G1048576 G23:G24 G18:G21">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="G2:G17 G27 G29:G1048576 G24:G25 G19:G22">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="percent" val="80"/>
         <cfvo type="percent" val="90"/>
@@ -2344,7 +2621,67 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M32:M1048576 M1:M30">
+  <conditionalFormatting sqref="M33:M1048576 M2:M31">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S3">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S29 S31:S1048576">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S30">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z4">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="percent" val="90"/>
@@ -2356,7 +2693,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3">
+  <conditionalFormatting sqref="Z4">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="percent" val="90"/>
+        <cfvo type="percent" val="95"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z4:Z35 Z37:Z1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="percent" val="90"/>
@@ -2368,7 +2717,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S2">
+  <conditionalFormatting sqref="Z2:Z3">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="percent" val="90"/>
@@ -2380,7 +2729,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S28 S30:S1048576">
+  <conditionalFormatting sqref="Z2:Z3">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="percent" val="90"/>
@@ -2392,7 +2741,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S29">
+  <conditionalFormatting sqref="Z36">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="90"/>
@@ -2410,6 +2759,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004955207F9F5B314B8B9B51B8E365D485" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c516aae3580213d3db2e32983502eaaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c1ef9b3-4174-4af3-a5b1-5f98b740a774" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c89a2e4264c97434fad65ccc84a3a390" ns2:_="">
     <xsd:import namespace="4c1ef9b3-4174-4af3-a5b1-5f98b740a774"/>
@@ -2557,7 +2912,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2566,13 +2921,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE5D3DB7-DCDC-44A8-A58C-499D0DB8587A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2590,19 +2948,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548F9C72-C66E-46A6-BA34-52C8707B9224}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9526D1D9-FB3C-467D-BC63-924F291A0DF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>